<commit_message>
Added Digi-Key prices to BOM.
Also added License to NXP.txt.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="399">
   <si>
     <t>BT1</t>
   </si>
@@ -1198,13 +1198,47 @@
   </si>
   <si>
     <t>SN65HVD1176DR</t>
+  </si>
+  <si>
+    <t>Cantidad para 100 PCBs</t>
+  </si>
+  <si>
+    <t>Costo de componentes:</t>
+  </si>
+  <si>
+    <t>Montaje:</t>
+  </si>
+  <si>
+    <t>PCB:</t>
+  </si>
+  <si>
+    <t>Gabinete:</t>
+  </si>
+  <si>
+    <t>Costo unitario (USD - DK)</t>
+  </si>
+  <si>
+    <t>aprox.</t>
+  </si>
+  <si>
+    <t>Costo unitario total:</t>
+  </si>
+  <si>
+    <t>(para 100 unidades)</t>
+  </si>
+  <si>
+    <t>aprox. (www.pcbcart.com)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1336,6 +1370,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1638,7 +1686,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1681,8 +1729,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1699,8 +1748,26 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1732,6 +1799,7 @@
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Moneda" xfId="42" builtinId="4"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
@@ -2038,23 +2106,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>119</v>
       </c>
@@ -2070,9 +2140,14 @@
       <c r="E1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>118</v>
       </c>
@@ -2088,8 +2163,15 @@
       <c r="E2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2">
+        <f>100*B2</f>
+        <v>100</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2105,8 +2187,15 @@
       <c r="E3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">100*B3</f>
+        <v>200</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1.21E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2122,8 +2211,15 @@
       <c r="E4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1.54E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2139,8 +2235,15 @@
       <c r="E5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1.38E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2156,8 +2259,15 @@
       <c r="E6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.38E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2173,8 +2283,15 @@
       <c r="E7" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1.652E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2190,8 +2307,15 @@
       <c r="E8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1.12E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
@@ -2207,8 +2331,15 @@
       <c r="E9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G9" s="10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -2224,8 +2355,15 @@
       <c r="E10" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>5800</v>
+      </c>
+      <c r="G10" s="10">
+        <v>5.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2241,8 +2379,15 @@
       <c r="E11" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.47E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2258,8 +2403,15 @@
       <c r="E12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G12" s="10">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2275,8 +2427,15 @@
       <c r="E13" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.40610000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -2292,8 +2451,15 @@
       <c r="E14" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.5169999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2309,8 +2475,15 @@
       <c r="E15" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="G15" s="10">
+        <v>8.6459999999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2326,8 +2499,15 @@
       <c r="E16" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.20752000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2343,8 +2523,15 @@
       <c r="E17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.46700000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>120</v>
       </c>
@@ -2360,8 +2547,15 @@
       <c r="E18" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.73440000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2377,8 +2571,15 @@
       <c r="E19" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G19" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -2394,8 +2595,15 @@
       <c r="E20" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.23832</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -2411,8 +2619,15 @@
       <c r="E21" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1.4829999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -2428,8 +2643,15 @@
       <c r="E22" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0.1158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2445,8 +2667,15 @@
       <c r="E23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="G23" s="10">
+        <v>2.5080000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
@@ -2462,8 +2691,15 @@
       <c r="E24" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G24" s="10">
+        <v>3.4840000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
         <v>136</v>
       </c>
@@ -2479,8 +2715,15 @@
       <c r="E25" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G25" s="10">
+        <v>3.4840000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -2496,8 +2739,15 @@
       <c r="E26" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G26" s="10">
+        <v>2.3561999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -2513,8 +2763,15 @@
       <c r="E27" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0.54449999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2530,8 +2787,15 @@
       <c r="E28" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.77439999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
         <v>141</v>
       </c>
@@ -2547,8 +2811,15 @@
       <c r="E29" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2564,8 +2835,15 @@
       <c r="E30" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
         <v>139</v>
       </c>
@@ -2581,8 +2859,15 @@
       <c r="E31" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -2598,8 +2883,15 @@
       <c r="E32" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G32" s="10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
         <v>372</v>
       </c>
@@ -2612,8 +2904,15 @@
       <c r="E33" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0.47039999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -2629,8 +2928,15 @@
       <c r="E34" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G34" s="10">
+        <v>1.98024</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -2646,8 +2952,15 @@
       <c r="E35" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -2663,8 +2976,15 @@
       <c r="E36" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G36" s="10">
+        <v>3.4799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
         <v>373</v>
       </c>
@@ -2680,8 +3000,15 @@
       <c r="E37" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G37" s="10">
+        <v>5.9089999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
         <v>374</v>
       </c>
@@ -2694,8 +3021,15 @@
       <c r="E38" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0.8337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
@@ -2711,8 +3045,15 @@
       <c r="E39" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -2728,8 +3069,15 @@
       <c r="E40" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0.22639999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
         <v>143</v>
       </c>
@@ -2745,8 +3093,15 @@
       <c r="E41" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0.2177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
         <v>144</v>
       </c>
@@ -2762,8 +3117,15 @@
       <c r="E42" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G42" s="10">
+        <v>7.9699999999999993E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
@@ -2779,8 +3141,15 @@
       <c r="E43" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G43" s="10">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -2796,8 +3165,15 @@
       <c r="E44" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0.11541999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1">
       <c r="A45" s="2">
         <v>0</v>
       </c>
@@ -2813,8 +3189,15 @@
       <c r="E45" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="G45" s="10">
+        <v>2.0400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>4.7</v>
       </c>
@@ -2830,8 +3213,15 @@
       <c r="E46" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G46" s="10">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>22</v>
       </c>
@@ -2847,8 +3237,15 @@
       <c r="E47" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G47" s="10">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
         <v>376</v>
       </c>
@@ -2864,8 +3261,15 @@
       <c r="E48" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0.2823</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>50</v>
       </c>
@@ -2881,8 +3285,15 @@
       <c r="E49" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G49" s="10">
+        <v>4.5599999999999998E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>60</v>
       </c>
@@ -2898,8 +3309,15 @@
       <c r="E50" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G50" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>100</v>
       </c>
@@ -2915,8 +3333,15 @@
       <c r="E51" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G51" s="10">
+        <v>2.0400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>120</v>
       </c>
@@ -2932,8 +3357,15 @@
       <c r="E52" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G52" s="10">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
         <v>378</v>
       </c>
@@ -2949,8 +3381,15 @@
       <c r="E53" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G53" s="10">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>270</v>
       </c>
@@ -2966,8 +3405,15 @@
       <c r="E54" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G54" s="10">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>330</v>
       </c>
@@ -2983,8 +3429,15 @@
       <c r="E55" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="G55" s="10">
+        <v>2.7799999999999999E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>680</v>
       </c>
@@ -3000,8 +3453,15 @@
       <c r="E56" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G56" s="10">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
         <v>60</v>
       </c>
@@ -3017,8 +3477,15 @@
       <c r="E57" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G57" s="10">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
         <v>149</v>
       </c>
@@ -3034,8 +3501,15 @@
       <c r="E58" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G58" s="10">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>62</v>
       </c>
@@ -3051,8 +3525,15 @@
       <c r="E59" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G59" s="10">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
         <v>381</v>
       </c>
@@ -3068,8 +3549,15 @@
       <c r="E60" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G60" s="10">
+        <v>0.1434</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -3085,8 +3573,15 @@
       <c r="E61" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="30">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G61" s="10">
+        <v>2.7799999999999999E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30">
       <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
@@ -3102,8 +3597,15 @@
       <c r="E62" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G62" s="10">
+        <v>1.7700000000000001E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="2" t="s">
         <v>151</v>
       </c>
@@ -3119,8 +3621,15 @@
       <c r="E63" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G63" s="10">
+        <v>4.5599999999999998E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -3136,8 +3645,15 @@
       <c r="E64" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G64" s="10">
+        <v>7.4609999999999996E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="2" t="s">
         <v>152</v>
       </c>
@@ -3153,8 +3669,15 @@
       <c r="E65" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G65" s="10">
+        <v>0.1434</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
@@ -3170,8 +3693,15 @@
       <c r="E66" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="G66" s="10">
+        <v>2.0400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -3187,8 +3717,15 @@
       <c r="E67" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <f t="shared" ref="F67:F100" si="1">100*B67</f>
+        <v>100</v>
+      </c>
+      <c r="G67" s="10">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -3204,8 +3741,15 @@
       <c r="E68" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G68" s="10">
+        <v>0.13780000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
@@ -3221,8 +3765,15 @@
       <c r="E69" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G69" s="10">
+        <v>0.15820000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
         <v>154</v>
       </c>
@@ -3238,8 +3789,15 @@
       <c r="E70" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="G70" s="10">
+        <v>0.14244999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
         <v>156</v>
       </c>
@@ -3255,8 +3813,15 @@
       <c r="E71" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G71" s="10">
+        <v>0.22639999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
@@ -3272,8 +3837,15 @@
       <c r="E72" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G72" s="10">
+        <v>0.4158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
@@ -3289,8 +3861,15 @@
       <c r="E73" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="G73" s="10">
+        <v>0.16800000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
@@ -3306,8 +3885,15 @@
       <c r="E74" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G74" s="10">
+        <v>0.24260000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="2" t="s">
         <v>159</v>
       </c>
@@ -3323,8 +3909,15 @@
       <c r="E75" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="G75" s="10">
+        <v>0.29924000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -3340,8 +3933,15 @@
       <c r="E76" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G76" s="10">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
@@ -3357,8 +3957,15 @@
       <c r="E77" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G77" s="10">
+        <v>0.71819999999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="2" t="s">
         <v>82</v>
       </c>
@@ -3374,8 +3981,15 @@
       <c r="E78" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G78" s="10">
+        <v>0.92330000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="2" t="s">
         <v>84</v>
       </c>
@@ -3391,8 +4005,15 @@
       <c r="E79" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G79" s="10">
+        <v>0.25369999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="2" t="s">
         <v>86</v>
       </c>
@@ -3408,8 +4029,15 @@
       <c r="E80" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G80" s="10">
+        <v>0.7671</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
         <v>88</v>
       </c>
@@ -3425,8 +4053,15 @@
       <c r="E81" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G81" s="10">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="2" t="s">
         <v>123</v>
       </c>
@@ -3442,8 +4077,15 @@
       <c r="E82" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G82" s="10">
+        <v>2.6749999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="2" t="s">
         <v>162</v>
       </c>
@@ -3459,8 +4101,15 @@
       <c r="E83" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G83" s="10">
+        <v>0.26519999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="2" t="s">
         <v>91</v>
       </c>
@@ -3476,8 +4125,15 @@
       <c r="E84" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G84" s="10">
+        <v>1.6704000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="2" t="s">
         <v>93</v>
       </c>
@@ -3493,8 +4149,15 @@
       <c r="E85" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G85" s="10">
+        <v>2.4119999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -3510,8 +4173,15 @@
       <c r="E86" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G86" s="10">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="2" t="s">
         <v>163</v>
       </c>
@@ -3527,8 +4197,15 @@
       <c r="E87" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G87" s="10">
+        <v>0.26050000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="2" t="s">
         <v>165</v>
       </c>
@@ -3544,8 +4221,15 @@
       <c r="E88" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G88" s="10">
+        <v>0.20860000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="2" t="s">
         <v>388</v>
       </c>
@@ -3561,8 +4245,15 @@
       <c r="E89" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G89" s="10">
+        <v>3.1017000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
@@ -3578,8 +4269,15 @@
       <c r="E90" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G90" s="10">
+        <v>1.0017</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="2" t="s">
         <v>166</v>
       </c>
@@ -3595,8 +4293,15 @@
       <c r="E91" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G91" s="10">
+        <v>3.4182000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -3612,8 +4317,15 @@
       <c r="E92" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G92" s="10">
+        <v>0.31269999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="2" t="s">
         <v>103</v>
       </c>
@@ -3629,8 +4341,15 @@
       <c r="E93" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G93" s="10">
+        <v>0.35780000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="2" t="s">
         <v>105</v>
       </c>
@@ -3646,8 +4365,15 @@
       <c r="E94" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G94" s="10">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="2" t="s">
         <v>168</v>
       </c>
@@ -3663,8 +4389,15 @@
       <c r="E95" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G95" s="10">
+        <v>0.4985</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
         <v>107</v>
       </c>
@@ -3680,8 +4413,15 @@
       <c r="E96" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G96" s="10">
+        <v>0.432</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="2" t="s">
         <v>109</v>
       </c>
@@ -3697,8 +4437,15 @@
       <c r="E97" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="G97" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="2" t="s">
         <v>111</v>
       </c>
@@ -3714,8 +4461,15 @@
       <c r="E98" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="G98" s="10">
+        <v>0.24968000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="2" t="s">
         <v>113</v>
       </c>
@@ -3731,8 +4485,15 @@
       <c r="E99" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="G99" s="10">
+        <v>0.22992000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="2" t="s">
         <v>114</v>
       </c>
@@ -3747,6 +4508,67 @@
       </c>
       <c r="E100" t="s">
         <v>368</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G100" s="10">
+        <v>0.12470000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="F101" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="G101" s="10">
+        <f>SUM(G2:G100)</f>
+        <v>63.511639999999993</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="F103" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="G103" s="11">
+        <v>5</v>
+      </c>
+      <c r="H103" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="F104" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="G104" s="13">
+        <v>5.7</v>
+      </c>
+      <c r="H104" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="F105" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="G105" s="11">
+        <v>5</v>
+      </c>
+      <c r="H105" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="F107" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="G107" s="8">
+        <f>SUM(G103:G105,G101)</f>
+        <v>79.211639999999989</v>
+      </c>
+      <c r="H107" s="12" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM updated with pluggable terminal blocks.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -10,7 +10,7 @@
     <sheet name="ciaa-nxp" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ciaa_nxp_1" localSheetId="0">'ciaa-nxp'!$A$2:$C$100</definedName>
+    <definedName name="ciaa_nxp_1" localSheetId="0">'ciaa-nxp'!$A$2:$C$104</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="408">
   <si>
     <t>BT1</t>
   </si>
@@ -1228,6 +1228,33 @@
   </si>
   <si>
     <t>aprox. (www.pcbcart.com)</t>
+  </si>
+  <si>
+    <t>TBP_1X8</t>
+  </si>
+  <si>
+    <t>TBP_1X4</t>
+  </si>
+  <si>
+    <t>TBH_1X8</t>
+  </si>
+  <si>
+    <t>Borneras enchufables alternativas (bornes)</t>
+  </si>
+  <si>
+    <t>Borneras enchufables alternativas (header)</t>
+  </si>
+  <si>
+    <t>277-1101-ND</t>
+  </si>
+  <si>
+    <t>ED1723-ND</t>
+  </si>
+  <si>
+    <t>ED2910-ND</t>
+  </si>
+  <si>
+    <t>A98067-ND</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1263,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1755,15 +1782,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2106,10 +2133,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <pane ySplit="9000" topLeftCell="A111"/>
+      <selection activeCell="H38" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2188,7 +2217,7 @@
         <v>176</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">100*B3</f>
+        <f t="shared" ref="F3:F35" si="0">100*B3</f>
         <v>200</v>
       </c>
       <c r="G3" s="10">
@@ -2339,7 +2368,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45">
+    <row r="10" spans="1:7" ht="75">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -2507,7 +2536,7 @@
         <v>0.20752000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>120</v>
       </c>
@@ -2555,7 +2584,7 @@
         <v>0.73440000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:8" ht="30">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2579,7 +2608,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -2603,7 +2632,7 @@
         <v>0.23832</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8" ht="30">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -2627,7 +2656,7 @@
         <v>1.4829999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -2651,7 +2680,7 @@
         <v>0.1158</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2675,7 +2704,7 @@
         <v>2.5080000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
         <v>134</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>3.4840000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>136</v>
       </c>
@@ -2723,7 +2752,7 @@
         <v>3.4840000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -2747,7 +2776,7 @@
         <v>2.3561999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -2771,7 +2800,7 @@
         <v>0.54449999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2795,7 +2824,7 @@
         <v>0.77439999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
         <v>141</v>
       </c>
@@ -2819,7 +2848,7 @@
         <v>0.72599999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2843,7 +2872,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>139</v>
       </c>
@@ -2867,595 +2896,583 @@
         <v>0.23100000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>371</v>
+        <v>402</v>
       </c>
       <c r="D32" t="s">
-        <v>233</v>
-      </c>
-      <c r="E32" t="s">
-        <v>234</v>
+        <v>405</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="G32" s="10">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>400</v>
+      </c>
+      <c r="H32" s="10">
+        <v>3.0362399999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>372</v>
+        <v>400</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="D33" t="s">
-        <v>235</v>
-      </c>
-      <c r="E33" t="s">
-        <v>236</v>
+        <v>406</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G33" s="10">
-        <v>0.47039999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="10">
+        <v>1.1970000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>401</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>403</v>
       </c>
       <c r="D34" t="s">
-        <v>237</v>
-      </c>
-      <c r="E34" t="s">
-        <v>238</v>
+        <v>407</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="G34" s="10">
-        <v>1.98024</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="10">
+        <v>1.8673999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>401</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>403</v>
       </c>
       <c r="D35" t="s">
-        <v>239</v>
-      </c>
-      <c r="E35" t="s">
-        <v>240</v>
+        <v>404</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G35" s="10">
+        <v>200</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D36" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36">
+        <f>100*B36</f>
+        <v>1500</v>
+      </c>
+      <c r="G36" s="10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>235</v>
+      </c>
+      <c r="E37" t="s">
+        <v>236</v>
+      </c>
+      <c r="F37">
+        <f>100*B37</f>
+        <v>200</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.47039999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>237</v>
+      </c>
+      <c r="E38" t="s">
+        <v>238</v>
+      </c>
+      <c r="F38">
+        <f>100*B38</f>
+        <v>400</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1.98024</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E39" t="s">
+        <v>240</v>
+      </c>
+      <c r="F39">
+        <f>100*B39</f>
+        <v>100</v>
+      </c>
+      <c r="G39" s="10">
         <v>0.45</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D40" t="s">
         <v>241</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E40" t="s">
         <v>242</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G36" s="10">
+      <c r="F40">
+        <f>100*B40</f>
+        <v>100</v>
+      </c>
+      <c r="G40" s="10">
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
+    <row r="41" spans="1:8">
+      <c r="A41" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>243</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E41" t="s">
         <v>244</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G37" s="10">
+      <c r="F41">
+        <f>100*B41</f>
+        <v>100</v>
+      </c>
+      <c r="G41" s="10">
         <v>5.9089999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
+    <row r="42" spans="1:8">
+      <c r="A42" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
         <v>245</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E42" t="s">
         <v>246</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G38" s="10">
+      <c r="F42">
+        <f>100*B42</f>
+        <v>100</v>
+      </c>
+      <c r="G42" s="10">
         <v>0.8337</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="2" t="s">
+    <row r="43" spans="1:8">
+      <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D43" t="s">
         <v>247</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E43" t="s">
         <v>248</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G39" s="10">
+      <c r="F43">
+        <f>100*B43</f>
+        <v>100</v>
+      </c>
+      <c r="G43" s="10">
         <v>0.88</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="2" t="s">
+    <row r="44" spans="1:8">
+      <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B40">
+      <c r="B44">
         <v>2</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D44" t="s">
         <v>249</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E44" t="s">
         <v>250</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
+      <c r="F44">
+        <f>100*B44</f>
         <v>200</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G44" s="10">
         <v>0.22639999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
+    <row r="45" spans="1:8" ht="15" customHeight="1">
+      <c r="A45" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D45" t="s">
         <v>253</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E45" t="s">
         <v>254</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G41" s="10">
+      <c r="F45">
+        <f>100*B45</f>
+        <v>100</v>
+      </c>
+      <c r="G45" s="10">
         <v>0.2177</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="2" t="s">
+    <row r="46" spans="1:8">
+      <c r="A46" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D46" t="s">
         <v>251</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E46" t="s">
         <v>252</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G42" s="10">
+      <c r="F46">
+        <f>100*B46</f>
+        <v>100</v>
+      </c>
+      <c r="G46" s="10">
         <v>7.9699999999999993E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="2" t="s">
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B43">
+      <c r="B47">
         <v>4</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D47" t="s">
         <v>255</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E47" t="s">
         <v>256</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
+      <c r="F47">
+        <f>100*B47</f>
         <v>400</v>
       </c>
-      <c r="G43" s="10">
+      <c r="G47" s="10">
         <v>1.006</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="2" t="s">
+    <row r="48" spans="1:8">
+      <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B44">
+      <c r="B48">
         <v>8</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D48" t="s">
         <v>257</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E48" t="s">
         <v>258</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="0"/>
+      <c r="F48">
+        <f>100*B48</f>
         <v>800</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G48" s="10">
         <v>0.11541999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1">
-      <c r="A45" s="2">
+    <row r="49" spans="1:7" ht="30">
+      <c r="A49" s="2">
         <v>0</v>
       </c>
-      <c r="B45">
+      <c r="B49">
         <v>17</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D49" t="s">
         <v>259</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E49" t="s">
         <v>260</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
+      <c r="F49">
+        <f>100*B49</f>
         <v>1700</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G49" s="10">
         <v>2.0400000000000001E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="2">
-        <v>4.7</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" t="s">
-        <v>261</v>
-      </c>
-      <c r="E46" t="s">
-        <v>262</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="G46" s="10">
-        <v>3.48E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="2">
-        <v>22</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D47" t="s">
-        <v>263</v>
-      </c>
-      <c r="E47" t="s">
-        <v>264</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="G47" s="10">
-        <v>3.48E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B48">
-        <v>2</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D48" t="s">
-        <v>265</v>
-      </c>
-      <c r="E48" t="s">
-        <v>266</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="G48" s="10">
-        <v>0.2823</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="2">
-        <v>50</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" t="s">
-        <v>267</v>
-      </c>
-      <c r="E49" t="s">
-        <v>268</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="G49" s="10">
-        <v>4.5599999999999998E-3</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2">
-        <v>60</v>
+        <v>4.7</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E50" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
-        <v>200</v>
+        <f>100*B50</f>
+        <v>400</v>
       </c>
       <c r="G50" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>3.48E-3</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>377</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E51" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
-        <v>1200</v>
+        <f>100*B51</f>
+        <v>300</v>
       </c>
       <c r="G51" s="10">
-        <v>2.0400000000000001E-3</v>
+        <v>3.48E-3</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="2">
-        <v>120</v>
+      <c r="A52" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>58</v>
+        <v>375</v>
       </c>
       <c r="D52" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="E52" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>100*B52</f>
+        <v>200</v>
       </c>
       <c r="G52" s="10">
-        <v>4.4999999999999997E-3</v>
+        <v>0.2823</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="2" t="s">
-        <v>378</v>
+      <c r="A53" s="2">
+        <v>50</v>
       </c>
       <c r="B53">
         <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E53" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
+        <f>100*B53</f>
         <v>400</v>
       </c>
       <c r="G53" s="10">
-        <v>0.11</v>
+        <v>4.5599999999999998E-3</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2">
+        <v>60</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" t="s">
+        <v>269</v>
+      </c>
+      <c r="E54" t="s">
         <v>270</v>
       </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D54" t="s">
-        <v>277</v>
-      </c>
-      <c r="E54" t="s">
-        <v>278</v>
-      </c>
       <c r="F54">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>100*B54</f>
+        <v>200</v>
       </c>
       <c r="G54" s="10">
-        <v>3.48E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2">
-        <v>330</v>
+        <v>100</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>147</v>
+        <v>377</v>
       </c>
       <c r="D55" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="E55" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>800</v>
+        <f>100*B55</f>
+        <v>1200</v>
       </c>
       <c r="G55" s="10">
-        <v>2.7799999999999999E-3</v>
+        <v>2.0400000000000001E-3</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2">
-        <v>680</v>
+        <v>120</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="D56" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E56" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>200</v>
+        <f>100*B56</f>
+        <v>100</v>
       </c>
       <c r="G56" s="10">
         <v>4.4999999999999997E-3</v>
@@ -3463,1086 +3480,1157 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
-        <v>60</v>
+        <v>378</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D57" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E57" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
-        <v>200</v>
+        <f>100*B57</f>
+        <v>400</v>
       </c>
       <c r="G57" s="10">
-        <v>4.4999999999999997E-3</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="2" t="s">
-        <v>149</v>
+      <c r="A58" s="2">
+        <v>270</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>121</v>
+        <v>379</v>
       </c>
       <c r="D58" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E58" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>100*B58</f>
+        <v>400</v>
       </c>
       <c r="G58" s="10">
         <v>3.48E-3</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="2" t="s">
-        <v>62</v>
+      <c r="A59" s="2">
+        <v>330</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>380</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="E59" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>100*B59</f>
+        <v>800</v>
       </c>
       <c r="G59" s="10">
-        <v>3.48E-3</v>
+        <v>2.7799999999999999E-3</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="2" t="s">
-        <v>381</v>
+      <c r="A60" s="2">
+        <v>680</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E60" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>100*B60</f>
+        <v>200</v>
       </c>
       <c r="G60" s="10">
-        <v>0.1434</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E61" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <f>100*B61</f>
+        <v>200</v>
       </c>
       <c r="G61" s="10">
-        <v>2.7799999999999999E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="2" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B62">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>382</v>
+        <v>121</v>
       </c>
       <c r="D62" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E62" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
-        <v>2500</v>
+        <f>100*B62</f>
+        <v>300</v>
       </c>
       <c r="G62" s="10">
-        <v>1.7700000000000001E-3</v>
+        <v>3.48E-3</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="2" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D63" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E63" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>100*B63</f>
+        <v>400</v>
       </c>
       <c r="G63" s="10">
-        <v>4.5599999999999998E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="30">
+        <v>3.48E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>381</v>
       </c>
       <c r="B64">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>384</v>
+        <v>150</v>
       </c>
       <c r="D64" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E64" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <f>100*B64</f>
+        <v>100</v>
       </c>
       <c r="G64" s="10">
-        <v>7.4609999999999996E-2</v>
+        <v>0.1434</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="2" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E65" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>100*B65</f>
+        <v>500</v>
       </c>
       <c r="G65" s="10">
-        <v>0.1434</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>2.7799999999999999E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="45">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>122</v>
+        <v>382</v>
       </c>
       <c r="D66" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E66" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>1100</v>
+        <f>100*B66</f>
+        <v>2500</v>
       </c>
       <c r="G66" s="10">
-        <v>2.0400000000000001E-3</v>
+        <v>1.7700000000000001E-3</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>69</v>
+        <v>383</v>
       </c>
       <c r="D67" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E67" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F100" si="1">100*B67</f>
-        <v>100</v>
+        <f>100*B67</f>
+        <v>300</v>
       </c>
       <c r="G67" s="10">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>4.5599999999999998E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30">
       <c r="A68" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>71</v>
+        <v>384</v>
       </c>
       <c r="D68" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E68" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F68">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>100*B68</f>
+        <v>1500</v>
       </c>
       <c r="G68" s="10">
-        <v>0.13780000000000001</v>
+        <v>7.4609999999999996E-2</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" t="s">
+        <v>299</v>
+      </c>
+      <c r="E69" t="s">
+        <v>300</v>
+      </c>
+      <c r="F69">
+        <f>100*B69</f>
+        <v>100</v>
+      </c>
+      <c r="G69" s="10">
+        <v>0.1434</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="30">
+      <c r="A70" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>11</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D70" t="s">
+        <v>301</v>
+      </c>
+      <c r="E70" t="s">
+        <v>302</v>
+      </c>
+      <c r="F70">
+        <f>100*B70</f>
+        <v>1100</v>
+      </c>
+      <c r="G70" s="10">
+        <v>2.0400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" t="s">
+        <v>303</v>
+      </c>
+      <c r="E71" t="s">
+        <v>304</v>
+      </c>
+      <c r="F71">
+        <f t="shared" ref="F71:F104" si="1">100*B71</f>
+        <v>100</v>
+      </c>
+      <c r="G71" s="10">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" t="s">
+        <v>305</v>
+      </c>
+      <c r="E72" t="s">
+        <v>306</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G72" s="10">
+        <v>0.13780000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D73" t="s">
         <v>307</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E73" t="s">
         <v>308</v>
       </c>
-      <c r="F69">
+      <c r="F73">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G69" s="10">
+      <c r="G73" s="10">
         <v>0.15820000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="2" t="s">
+    <row r="74" spans="1:7">
+      <c r="A74" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B70">
+      <c r="B74">
         <v>12</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D74" t="s">
         <v>309</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E74" t="s">
         <v>310</v>
       </c>
-      <c r="F70">
+      <c r="F74">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="G70" s="10">
+      <c r="G74" s="10">
         <v>0.14244999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="2" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D75" t="s">
         <v>317</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E75" t="s">
         <v>318</v>
       </c>
-      <c r="F71">
+      <c r="F75">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G71" s="10">
+      <c r="G75" s="10">
         <v>0.22639999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="2" t="s">
+    <row r="76" spans="1:7">
+      <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1" t="s">
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D76" t="s">
         <v>311</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E76" t="s">
         <v>312</v>
       </c>
-      <c r="F72">
+      <c r="F76">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G72" s="10">
+      <c r="G76" s="10">
         <v>0.4158</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="2" t="s">
+    <row r="77" spans="1:7">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B73">
+      <c r="B77">
         <v>7</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D77" t="s">
         <v>313</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E77" t="s">
         <v>314</v>
       </c>
-      <c r="F73">
+      <c r="F77">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="G73" s="10">
+      <c r="G77" s="10">
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="2" t="s">
+    <row r="78" spans="1:7">
+      <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D78" t="s">
         <v>315</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E78" t="s">
         <v>316</v>
       </c>
-      <c r="F74">
+      <c r="F78">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G74" s="10">
+      <c r="G78" s="10">
         <v>0.24260000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="2" t="s">
+    <row r="79" spans="1:7">
+      <c r="A79" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B75">
+      <c r="B79">
         <v>3</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D79" t="s">
         <v>319</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E79" t="s">
         <v>320</v>
       </c>
-      <c r="F75">
+      <c r="F79">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="G75" s="10">
+      <c r="G79" s="10">
         <v>0.29924000000000001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" t="s">
-        <v>321</v>
-      </c>
-      <c r="E76" t="s">
-        <v>322</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G76" s="10">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" t="s">
-        <v>323</v>
-      </c>
-      <c r="E77" t="s">
-        <v>324</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G77" s="10">
-        <v>0.71819999999999995</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D78" t="s">
-        <v>325</v>
-      </c>
-      <c r="E78" t="s">
-        <v>326</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G78" s="10">
-        <v>0.92330000000000001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D79" t="s">
-        <v>327</v>
-      </c>
-      <c r="E79" t="s">
-        <v>328</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G79" s="10">
-        <v>0.25369999999999998</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E80" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="F80">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G80" s="10">
-        <v>0.7671</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E81" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="F81">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G81" s="10">
-        <v>1.44</v>
+        <v>0.71819999999999995</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="2" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="D82" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E82" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F82">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G82" s="10">
-        <v>2.6749999999999998</v>
+        <v>0.92330000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="2" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D83" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E83" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="F83">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G83" s="10">
-        <v>0.26519999999999999</v>
+        <v>0.25369999999999998</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D84" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E84" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F84">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G84" s="10">
-        <v>1.6704000000000001</v>
+        <v>0.7671</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D85" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E85" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="F85">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G85" s="10">
-        <v>2.4119999999999999</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="2" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="D86" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E86" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="F86">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G86" s="10">
-        <v>5.4</v>
+        <v>2.6749999999999998</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="D87" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E87" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="F87">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G87" s="10">
-        <v>0.26050000000000001</v>
+        <v>0.26519999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="2" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D88" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E88" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F88">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G88" s="10">
-        <v>0.20860000000000001</v>
+        <v>1.6704000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="2" t="s">
-        <v>388</v>
+        <v>93</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D89" t="s">
-        <v>386</v>
+        <v>339</v>
       </c>
       <c r="E89" t="s">
-        <v>387</v>
+        <v>340</v>
       </c>
       <c r="F89">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G89" s="10">
-        <v>3.1017000000000001</v>
+        <v>2.4119999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B90">
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D90" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E90" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F90">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G90" s="10">
-        <v>1.0017</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="D91" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E91" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F91">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G91" s="10">
-        <v>3.4182000000000001</v>
+        <v>0.26050000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
-        <v>97</v>
+        <v>165</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="D92" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E92" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F92">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G92" s="10">
-        <v>0.31269999999999998</v>
+        <v>0.20860000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="2" t="s">
-        <v>103</v>
+        <v>388</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D93" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="E93" t="s">
-        <v>354</v>
+        <v>387</v>
       </c>
       <c r="F93">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G93" s="10">
-        <v>0.35780000000000001</v>
+        <v>3.1017000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D94" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E94" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F94">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G94" s="10">
-        <v>11.05</v>
+        <v>1.0017</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="D95" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E95" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="F95">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G95" s="10">
-        <v>0.4985</v>
+        <v>3.4182000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="D96" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="E96" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F96">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G96" s="10">
-        <v>0.432</v>
+        <v>0.31269999999999998</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D97" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E97" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="F97">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G97" s="10">
-        <v>0.8</v>
+        <v>0.35780000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B98">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D98" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E98" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F98">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="G98" s="10">
-        <v>0.24968000000000001</v>
+        <v>11.05</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="2" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="B99">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D99" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E99" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="F99">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>100</v>
       </c>
       <c r="G99" s="10">
-        <v>0.22992000000000001</v>
+        <v>0.4985</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D100" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E100" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="F100">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G100" s="10">
-        <v>0.12470000000000001</v>
+        <v>0.432</v>
       </c>
     </row>
     <row r="101" spans="1:8">
-      <c r="F101" s="6" t="s">
-        <v>390</v>
+      <c r="A101" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D101" t="s">
+        <v>361</v>
+      </c>
+      <c r="E101" t="s">
+        <v>362</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
       <c r="G101" s="10">
-        <f>SUM(G2:G100)</f>
-        <v>63.511639999999993</v>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D102" t="s">
+        <v>363</v>
+      </c>
+      <c r="E102" t="s">
+        <v>364</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="G102" s="10">
+        <v>0.24968000000000001</v>
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="F103" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="G103" s="11">
-        <v>5</v>
+      <c r="A103" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D103" t="s">
+        <v>365</v>
+      </c>
+      <c r="E103" t="s">
+        <v>366</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="G103" s="10">
+        <v>0.22992000000000001</v>
       </c>
       <c r="H103" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="104" spans="1:8">
-      <c r="F104" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="G104" s="13">
-        <v>5.7</v>
+      <c r="A104" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" t="s">
+        <v>367</v>
+      </c>
+      <c r="E104" t="s">
+        <v>368</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G104" s="10">
+        <v>0.12470000000000001</v>
       </c>
       <c r="H104" t="s">
         <v>398</v>
@@ -4550,25 +4638,50 @@
     </row>
     <row r="105" spans="1:8">
       <c r="F105" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="G105" s="11">
-        <v>5</v>
+        <v>390</v>
+      </c>
+      <c r="G105" s="10">
+        <f>SUM(G2:G104)</f>
+        <v>63.511639999999993</v>
       </c>
       <c r="H105" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="107" spans="1:8">
-      <c r="F107" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="G107" s="8">
-        <f>SUM(G103:G105,G101)</f>
-        <v>79.211639999999989</v>
+      <c r="F107" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="G107" s="11">
+        <v>5</v>
       </c>
       <c r="H107" s="12" t="s">
         <v>397</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="F108" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="G108" s="13">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="F109" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="G109" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="F111" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="G111" s="8">
+        <f>SUM(G107:G109,G105)</f>
+        <v>79.211639999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected format error in BOM.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -2135,11 +2135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <pane ySplit="9000" topLeftCell="A111"/>
-      <selection activeCell="H38" sqref="H38"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2997,7 +2993,7 @@
         <v>234</v>
       </c>
       <c r="F36">
-        <f>100*B36</f>
+        <f t="shared" ref="F36:F70" si="1">100*B36</f>
         <v>1500</v>
       </c>
       <c r="G36" s="10">
@@ -3018,7 +3014,7 @@
         <v>236</v>
       </c>
       <c r="F37">
-        <f>100*B37</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G37" s="10">
@@ -3042,7 +3038,7 @@
         <v>238</v>
       </c>
       <c r="F38">
-        <f>100*B38</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G38" s="10">
@@ -3066,7 +3062,7 @@
         <v>240</v>
       </c>
       <c r="F39">
-        <f>100*B39</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G39" s="10">
@@ -3090,7 +3086,7 @@
         <v>242</v>
       </c>
       <c r="F40">
-        <f>100*B40</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G40" s="10">
@@ -3114,7 +3110,7 @@
         <v>244</v>
       </c>
       <c r="F41">
-        <f>100*B41</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G41" s="10">
@@ -3135,7 +3131,7 @@
         <v>246</v>
       </c>
       <c r="F42">
-        <f>100*B42</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G42" s="10">
@@ -3159,7 +3155,7 @@
         <v>248</v>
       </c>
       <c r="F43">
-        <f>100*B43</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G43" s="10">
@@ -3183,7 +3179,7 @@
         <v>250</v>
       </c>
       <c r="F44">
-        <f>100*B44</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G44" s="10">
@@ -3207,7 +3203,7 @@
         <v>254</v>
       </c>
       <c r="F45">
-        <f>100*B45</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G45" s="10">
@@ -3231,7 +3227,7 @@
         <v>252</v>
       </c>
       <c r="F46">
-        <f>100*B46</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G46" s="10">
@@ -3255,7 +3251,7 @@
         <v>256</v>
       </c>
       <c r="F47">
-        <f>100*B47</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G47" s="10">
@@ -3279,7 +3275,7 @@
         <v>258</v>
       </c>
       <c r="F48">
-        <f>100*B48</f>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="G48" s="10">
@@ -3303,7 +3299,7 @@
         <v>260</v>
       </c>
       <c r="F49">
-        <f>100*B49</f>
+        <f t="shared" si="1"/>
         <v>1700</v>
       </c>
       <c r="G49" s="10">
@@ -3327,7 +3323,7 @@
         <v>262</v>
       </c>
       <c r="F50">
-        <f>100*B50</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G50" s="10">
@@ -3351,7 +3347,7 @@
         <v>264</v>
       </c>
       <c r="F51">
-        <f>100*B51</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="G51" s="10">
@@ -3375,7 +3371,7 @@
         <v>266</v>
       </c>
       <c r="F52">
-        <f>100*B52</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G52" s="10">
@@ -3399,7 +3395,7 @@
         <v>268</v>
       </c>
       <c r="F53">
-        <f>100*B53</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G53" s="10">
@@ -3423,7 +3419,7 @@
         <v>270</v>
       </c>
       <c r="F54">
-        <f>100*B54</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G54" s="10">
@@ -3447,7 +3443,7 @@
         <v>272</v>
       </c>
       <c r="F55">
-        <f>100*B55</f>
+        <f t="shared" si="1"/>
         <v>1200</v>
       </c>
       <c r="G55" s="10">
@@ -3471,7 +3467,7 @@
         <v>274</v>
       </c>
       <c r="F56">
-        <f>100*B56</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G56" s="10">
@@ -3495,7 +3491,7 @@
         <v>276</v>
       </c>
       <c r="F57">
-        <f>100*B57</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G57" s="10">
@@ -3519,7 +3515,7 @@
         <v>278</v>
       </c>
       <c r="F58">
-        <f>100*B58</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G58" s="10">
@@ -3543,7 +3539,7 @@
         <v>280</v>
       </c>
       <c r="F59">
-        <f>100*B59</f>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="G59" s="10">
@@ -3567,7 +3563,7 @@
         <v>282</v>
       </c>
       <c r="F60">
-        <f>100*B60</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G60" s="10">
@@ -3591,7 +3587,7 @@
         <v>284</v>
       </c>
       <c r="F61">
-        <f>100*B61</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G61" s="10">
@@ -3615,7 +3611,7 @@
         <v>286</v>
       </c>
       <c r="F62">
-        <f>100*B62</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="G62" s="10">
@@ -3639,7 +3635,7 @@
         <v>288</v>
       </c>
       <c r="F63">
-        <f>100*B63</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="G63" s="10">
@@ -3663,7 +3659,7 @@
         <v>290</v>
       </c>
       <c r="F64">
-        <f>100*B64</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G64" s="10">
@@ -3687,7 +3683,7 @@
         <v>292</v>
       </c>
       <c r="F65">
-        <f>100*B65</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="G65" s="10">
@@ -3711,7 +3707,7 @@
         <v>294</v>
       </c>
       <c r="F66">
-        <f>100*B66</f>
+        <f t="shared" si="1"/>
         <v>2500</v>
       </c>
       <c r="G66" s="10">
@@ -3735,7 +3731,7 @@
         <v>296</v>
       </c>
       <c r="F67">
-        <f>100*B67</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="G67" s="10">
@@ -3759,7 +3755,7 @@
         <v>298</v>
       </c>
       <c r="F68">
-        <f>100*B68</f>
+        <f t="shared" si="1"/>
         <v>1500</v>
       </c>
       <c r="G68" s="10">
@@ -3783,7 +3779,7 @@
         <v>300</v>
       </c>
       <c r="F69">
-        <f>100*B69</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G69" s="10">
@@ -3807,7 +3803,7 @@
         <v>302</v>
       </c>
       <c r="F70">
-        <f>100*B70</f>
+        <f t="shared" si="1"/>
         <v>1100</v>
       </c>
       <c r="G70" s="10">
@@ -3831,7 +3827,7 @@
         <v>304</v>
       </c>
       <c r="F71">
-        <f t="shared" ref="F71:F104" si="1">100*B71</f>
+        <f t="shared" ref="F71:F104" si="2">100*B71</f>
         <v>100</v>
       </c>
       <c r="G71" s="10">
@@ -3855,7 +3851,7 @@
         <v>306</v>
       </c>
       <c r="F72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G72" s="10">
@@ -3879,7 +3875,7 @@
         <v>308</v>
       </c>
       <c r="F73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G73" s="10">
@@ -3903,7 +3899,7 @@
         <v>310</v>
       </c>
       <c r="F74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="G74" s="10">
@@ -3927,7 +3923,7 @@
         <v>318</v>
       </c>
       <c r="F75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G75" s="10">
@@ -3951,7 +3947,7 @@
         <v>312</v>
       </c>
       <c r="F76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G76" s="10">
@@ -3975,7 +3971,7 @@
         <v>314</v>
       </c>
       <c r="F77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>700</v>
       </c>
       <c r="G77" s="10">
@@ -3999,7 +3995,7 @@
         <v>316</v>
       </c>
       <c r="F78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G78" s="10">
@@ -4023,7 +4019,7 @@
         <v>320</v>
       </c>
       <c r="F79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="G79" s="10">
@@ -4047,7 +4043,7 @@
         <v>322</v>
       </c>
       <c r="F80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G80" s="10">
@@ -4071,7 +4067,7 @@
         <v>324</v>
       </c>
       <c r="F81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G81" s="10">
@@ -4095,7 +4091,7 @@
         <v>326</v>
       </c>
       <c r="F82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G82" s="10">
@@ -4119,7 +4115,7 @@
         <v>328</v>
       </c>
       <c r="F83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G83" s="10">
@@ -4143,7 +4139,7 @@
         <v>330</v>
       </c>
       <c r="F84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G84" s="10">
@@ -4167,7 +4163,7 @@
         <v>332</v>
       </c>
       <c r="F85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G85" s="10">
@@ -4191,7 +4187,7 @@
         <v>334</v>
       </c>
       <c r="F86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G86" s="10">
@@ -4215,7 +4211,7 @@
         <v>336</v>
       </c>
       <c r="F87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G87" s="10">
@@ -4239,7 +4235,7 @@
         <v>338</v>
       </c>
       <c r="F88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G88" s="10">
@@ -4263,7 +4259,7 @@
         <v>340</v>
       </c>
       <c r="F89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G89" s="10">
@@ -4287,7 +4283,7 @@
         <v>342</v>
       </c>
       <c r="F90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G90" s="10">
@@ -4311,7 +4307,7 @@
         <v>344</v>
       </c>
       <c r="F91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G91" s="10">
@@ -4335,7 +4331,7 @@
         <v>346</v>
       </c>
       <c r="F92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G92" s="10">
@@ -4359,7 +4355,7 @@
         <v>387</v>
       </c>
       <c r="F93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G93" s="10">
@@ -4383,7 +4379,7 @@
         <v>348</v>
       </c>
       <c r="F94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G94" s="10">
@@ -4407,7 +4403,7 @@
         <v>350</v>
       </c>
       <c r="F95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G95" s="10">
@@ -4431,7 +4427,7 @@
         <v>352</v>
       </c>
       <c r="F96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G96" s="10">
@@ -4455,7 +4451,7 @@
         <v>354</v>
       </c>
       <c r="F97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G97" s="10">
@@ -4479,7 +4475,7 @@
         <v>356</v>
       </c>
       <c r="F98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G98" s="10">
@@ -4503,7 +4499,7 @@
         <v>358</v>
       </c>
       <c r="F99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G99" s="10">
@@ -4527,7 +4523,7 @@
         <v>360</v>
       </c>
       <c r="F100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G100" s="10">
@@ -4551,7 +4547,7 @@
         <v>362</v>
       </c>
       <c r="F101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="G101" s="10">
@@ -4575,7 +4571,7 @@
         <v>364</v>
       </c>
       <c r="F102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="G102" s="10">
@@ -4599,14 +4595,11 @@
         <v>366</v>
       </c>
       <c r="F103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>900</v>
       </c>
       <c r="G103" s="10">
         <v>0.22992000000000001</v>
-      </c>
-      <c r="H103" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4626,14 +4619,11 @@
         <v>368</v>
       </c>
       <c r="F104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G104" s="10">
         <v>0.12470000000000001</v>
-      </c>
-      <c r="H104" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4644,9 +4634,6 @@
         <f>SUM(G2:G104)</f>
         <v>63.511639999999993</v>
       </c>
-      <c r="H105" t="s">
-        <v>395</v>
-      </c>
     </row>
     <row r="107" spans="1:8">
       <c r="F107" s="6" t="s">
@@ -4655,8 +4642,8 @@
       <c r="G107" s="11">
         <v>5</v>
       </c>
-      <c r="H107" s="12" t="s">
-        <v>397</v>
+      <c r="H107" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4666,6 +4653,9 @@
       <c r="G108" s="13">
         <v>5.7</v>
       </c>
+      <c r="H108" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="109" spans="1:8">
       <c r="F109" s="6" t="s">
@@ -4674,6 +4664,9 @@
       <c r="G109" s="11">
         <v>5</v>
       </c>
+      <c r="H109" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="111" spans="1:8">
       <c r="F111" s="7" t="s">
@@ -4682,6 +4675,9 @@
       <c r="G111" s="8">
         <f>SUM(G107:G109,G105)</f>
         <v>79.211639999999989</v>
+      </c>
+      <c r="H111" s="12" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM: Corrected error in import fees formula.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="227" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="266" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ciaa-nxp" sheetId="1" state="visible" r:id="rId2"/>
@@ -1861,15 +1861,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>611640</xdr:colOff>
+      <xdr:colOff>612360</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1558440</xdr:colOff>
+      <xdr:colOff>1558800</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1878,8 +1878,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8129160" y="20527560"/>
-          <a:ext cx="2630880" cy="1233720"/>
+          <a:off x="8129880" y="20528280"/>
+          <a:ext cx="2630520" cy="1251720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1924,7 +1924,7 @@
   <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I105" activeCellId="0" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5868,8 +5868,8 @@
         <v>459</v>
       </c>
       <c r="I105" s="9" t="n">
-        <f aca="false">I104*(I101+I103)</f>
-        <v>40.302168</v>
+        <f aca="false">I104*(I101+I103/100)</f>
+        <v>28.422168</v>
       </c>
       <c r="J105" s="11"/>
     </row>
@@ -5913,7 +5913,7 @@
       <c r="H111" s="20"/>
       <c r="I111" s="21" t="n">
         <f aca="false">SUM(I107:I109,I101,I105,I103/100)</f>
-        <v>135.042728</v>
+        <v>123.162728</v>
       </c>
       <c r="J111" s="22"/>
     </row>
@@ -6109,8 +6109,8 @@
         <v>459</v>
       </c>
       <c r="I122" s="9" t="n">
-        <f aca="false">I104*(I119+I103)</f>
-        <v>46.242636</v>
+        <f aca="false">I104*(I119+I103/100)</f>
+        <v>34.362636</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6125,7 +6125,7 @@
       <c r="H124" s="20"/>
       <c r="I124" s="21" t="n">
         <f aca="false">SUM(I107:I109,I119,I122,I103/100)</f>
-        <v>160.784756</v>
+        <v>148.904756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM updated with latest changes. Part numbers updated: - 10mA current regulators. - MURS360T3G diode.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="482">
   <si>
     <t>Componente</t>
   </si>
@@ -142,7 +142,7 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>C88</t>
+    <t>C69 C88</t>
   </si>
   <si>
     <t>399-1091-1-ND</t>
@@ -154,7 +154,7 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C2 C3 C4 C6 C9 C10 C15 C19 C20 C22 C23 C24 C25 C26 C27 C29 C30 C32 C33 C35 C37 C39 C41 C43 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C61 C62 C63 C64 C65 C66 C67 C69 C70 C71 C72 C73 C74 C75 C76 C77 C86 C87 C90</t>
+    <t>C2 C3 C4 C6 C9 C10 C15 C19 C20 C22 C23 C24 C25 C26 C27 C29 C30 C32 C33 C35 C37 C39 C41 C43 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C61 C62 C63 C64 C65 C66 C67 C70 C71 C72 C73 C74 C75 C76 C77 C86 C87 C90</t>
   </si>
   <si>
     <t>399-1096-1-ND</t>
@@ -181,7 +181,7 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>C1 C5 C18 C31 C34 C60 C68 C78</t>
+    <t>C1 C5 C18 C31 C34 C60 C68 C78 C21 C28</t>
   </si>
   <si>
     <t>399-10116-1-ND</t>
@@ -205,16 +205,16 @@
     <t>647-UCW1E331MNL1GS</t>
   </si>
   <si>
-    <t>470uF</t>
+    <t>470uF/35V</t>
   </si>
   <si>
     <t>C16</t>
   </si>
   <si>
-    <t>493-7425-1-ND</t>
-  </si>
-  <si>
-    <t>667-EEV-FK1H471M</t>
+    <t>493-3961-1-ND</t>
+  </si>
+  <si>
+    <t>647-UCL1V471MNL1GS</t>
   </si>
   <si>
     <t>BAV199</t>
@@ -247,7 +247,7 @@
     <t>771-PMEG3020EH-T/R</t>
   </si>
   <si>
-    <t>RS3J-E3/57T</t>
+    <t>MURS360T3G</t>
   </si>
   <si>
     <t>D2</t>
@@ -406,7 +406,7 @@
     <t>ZX62-AB-5PA</t>
   </si>
   <si>
-    <t>J6 J7</t>
+    <t>J6</t>
   </si>
   <si>
     <t>Conector micro USB tipo AB</t>
@@ -421,10 +421,10 @@
     <t>ZX62-B-5PA</t>
   </si>
   <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>Conector micro USB tipo A</t>
+    <t>J7 P16</t>
+  </si>
+  <si>
+    <t>Conector micro USB tipo B</t>
   </si>
   <si>
     <t>H11634CT-ND</t>
@@ -445,7 +445,7 @@
     <t>ED2610-ND</t>
   </si>
   <si>
-    <t>571-7969493</t>
+    <t>FIX</t>
   </si>
   <si>
     <t>TB_1X2</t>
@@ -460,9 +460,6 @@
     <t>ED2609-ND</t>
   </si>
   <si>
-    <t>571-7969492</t>
-  </si>
-  <si>
     <t>JUMPER</t>
   </si>
   <si>
@@ -724,10 +721,10 @@
     <t>R35</t>
   </si>
   <si>
-    <t>311-120GRCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW0603-120-E3</t>
+    <t>311-220GRCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-220-E3</t>
   </si>
   <si>
     <t>237 0.1% 25ppm/°C</t>
@@ -763,10 +760,10 @@
     <t>R32 R39</t>
   </si>
   <si>
-    <t>311-680GRCT-ND</t>
-  </si>
-  <si>
-    <t>71-CRCW0603-680-E3</t>
+    <t>311-390GRCT-ND</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-390-E3</t>
   </si>
   <si>
     <t>1k</t>
@@ -832,7 +829,7 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R2 R15 R16 R48 R49 R64 R66 R68 R70 R72 R74 R76 R78 R85 R117 R118 R119 R120 R90 R91 R92 R101 R102 R103 R109</t>
+    <t>R2 R15 R16 R48 R49 R64 R66 R68 R70 R72 R74 R76 R78 R85 R117 R118 R119 R120 R91 R101 R102 R103 R109</t>
   </si>
   <si>
     <t>311-10KGRCT-ND</t>
@@ -880,7 +877,7 @@
     <t>100k</t>
   </si>
   <si>
-    <t>R21 R106 R108 R110 R111 R112 R114 R115 R116 R33 R38</t>
+    <t>R21 R106 R108 R110 R111 R112 R114 R115 R116 R33 R38 R90 R92</t>
   </si>
   <si>
     <t>311-100KGRCT-ND</t>
@@ -931,19 +928,19 @@
     <t>612-TL3301BF260QG</t>
   </si>
   <si>
-    <t>NSI45020T1G</t>
+    <t>NSI50010YT1G</t>
   </si>
   <si>
     <t>T1 T2 T3 T4 T5 T6 T7 T8 T9 T10 T11 T12</t>
   </si>
   <si>
-    <t>Current limiter 20mA</t>
-  </si>
-  <si>
-    <t>NSI45020T1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>863-NSI45020AT1G</t>
+    <t>Current limiter 10mA</t>
+  </si>
+  <si>
+    <t>NSI50010YT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>863-NSI50010YT1G</t>
   </si>
   <si>
     <t>MF-USMF005-2</t>
@@ -1581,7 +1578,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1604,6 +1601,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1679,7 +1682,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1717,6 +1720,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1861,15 +1868,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>612360</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:colOff>615240</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1558800</xdr:colOff>
+      <xdr:colOff>1541160</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1878,8 +1885,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8129880" y="20528280"/>
-          <a:ext cx="2630520" cy="1251720"/>
+          <a:off x="8132760" y="20530440"/>
+          <a:ext cx="2531880" cy="1508040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1919,12 +1926,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I105" activeCellId="0" sqref="I105"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1933,12 +1941,13 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.2914979757085"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="35.5344129554656"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="28.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="18.9392712550607"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.8663967611336"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="18.0607287449393"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.331983805668"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.2348178137652"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.9028340080972"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="4" width="13.2267206477733"/>
-    <col collapsed="false" hidden="true" max="11" min="10" style="2" width="0"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="18.0607287449393"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="17.331983805668"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="8.51417004048583"/>
   </cols>
   <sheetData>
@@ -2010,7 +2019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2088,7 +2097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2244,12 +2253,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -2267,14 +2276,14 @@
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">100*B9</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H9" s="9" t="n">
         <v>0.009</v>
       </c>
       <c r="I9" s="9" t="n">
         <f aca="false">B9*H9</f>
-        <v>0.009</v>
+        <v>0.018</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>41</v>
@@ -2288,7 +2297,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>44</v>
@@ -2306,14 +2315,14 @@
       </c>
       <c r="G10" s="2" t="n">
         <f aca="false">100*B10</f>
-        <v>5800</v>
+        <v>5700</v>
       </c>
       <c r="H10" s="9" t="n">
         <v>0.0054</v>
       </c>
       <c r="I10" s="9" t="n">
         <f aca="false">B10*H10</f>
-        <v>0.3132</v>
+        <v>0.3078</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>45</v>
@@ -2322,7 +2331,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2361,7 +2370,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -2400,7 +2409,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -2454,11 +2463,11 @@
       </c>
       <c r="E14" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J14,J14)</f>
-        <v>493-7425-1-ND</v>
+        <v>493-3961-1-ND</v>
       </c>
       <c r="F14" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K14,K14)</f>
-        <v>667-EEV-FK1H471M</v>
+        <v>647-UCL1V471MNL1GS</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">100*B14</f>
@@ -2478,7 +2487,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2556,7 +2565,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -2595,7 +2604,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>80</v>
       </c>
@@ -2985,12 +2994,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>128</v>
@@ -3008,14 +3017,14 @@
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">100*B28</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H28" s="9" t="n">
         <v>0.7744</v>
       </c>
       <c r="I28" s="9" t="n">
         <f aca="false">B28*H28</f>
-        <v>1.5488</v>
+        <v>0.7744</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>130</v>
@@ -3024,12 +3033,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>133</v>
@@ -3047,14 +3056,14 @@
       </c>
       <c r="G29" s="2" t="n">
         <f aca="false">100*B29</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H29" s="9" t="n">
         <v>0.726</v>
       </c>
       <c r="I29" s="9" t="n">
         <f aca="false">B29*H29</f>
-        <v>0.726</v>
+        <v>1.452</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>135</v>
@@ -3063,7 +3072,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>137</v>
       </c>
@@ -3080,9 +3089,9 @@
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J30,J30)</f>
         <v>ED2610-ND</v>
       </c>
-      <c r="F30" s="8" t="str">
+      <c r="F30" s="10" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K30,K30)</f>
-        <v>571-7969493</v>
+        <v>FIX</v>
       </c>
       <c r="G30" s="2" t="n">
         <f aca="false">100*B30</f>
@@ -3102,7 +3111,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>142</v>
       </c>
@@ -3119,9 +3128,9 @@
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J31,J31)</f>
         <v>ED2609-ND</v>
       </c>
-      <c r="F31" s="8" t="str">
+      <c r="F31" s="10" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K31,K31)</f>
-        <v>571-7969492</v>
+        <v>FIX</v>
       </c>
       <c r="G31" s="2" t="n">
         <f aca="false">100*B31</f>
@@ -3138,21 +3147,21 @@
         <v>145</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="E32" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J32,J32)</f>
@@ -3174,21 +3183,21 @@
         <v>0.63</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E33" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J33,J33)</f>
@@ -3210,24 +3219,24 @@
         <v>0.9408</v>
       </c>
       <c r="J33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="E34" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J34,J34)</f>
@@ -3249,24 +3258,24 @@
         <v>7.92096</v>
       </c>
       <c r="J34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="E35" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J35,J35)</f>
@@ -3288,24 +3297,24 @@
         <v>0.45</v>
       </c>
       <c r="J35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="E36" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J36,J36)</f>
@@ -3327,24 +3336,24 @@
         <v>0.0348</v>
       </c>
       <c r="J36" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E37" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J37,J37)</f>
@@ -3366,21 +3375,21 @@
         <v>5.909</v>
       </c>
       <c r="J37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="38" s="2" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E38" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J38,J38)</f>
@@ -3402,24 +3411,24 @@
         <v>0.8337</v>
       </c>
       <c r="J38" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E39" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J39,J39)</f>
@@ -3441,24 +3450,24 @@
         <v>0.88</v>
       </c>
       <c r="J39" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="E40" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J40,J40)</f>
@@ -3480,24 +3489,24 @@
         <v>0.4528</v>
       </c>
       <c r="J40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="E41" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J41,J41)</f>
@@ -3519,24 +3528,24 @@
         <v>0.2177</v>
       </c>
       <c r="J41" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="E42" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J42,J42)</f>
@@ -3558,24 +3567,24 @@
         <v>0.0797</v>
       </c>
       <c r="J42" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="E43" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J43,J43)</f>
@@ -3597,24 +3606,24 @@
         <v>4.024</v>
       </c>
       <c r="J43" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="E44" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J44,J44)</f>
@@ -3636,10 +3645,10 @@
         <v>0.92336</v>
       </c>
       <c r="J44" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3650,10 +3659,10 @@
         <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="E45" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J45,J45)</f>
@@ -3675,10 +3684,10 @@
         <v>0.03468</v>
       </c>
       <c r="J45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3689,10 +3698,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E46" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J46,J46)</f>
@@ -3714,10 +3723,10 @@
         <v>0.01392</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K46" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3728,10 +3737,10 @@
         <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E47" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J47,J47)</f>
@@ -3753,24 +3762,24 @@
         <v>0.01044</v>
       </c>
       <c r="J47" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K47" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E48" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J48,J48)</f>
@@ -3792,10 +3801,10 @@
         <v>0.5646</v>
       </c>
       <c r="J48" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,10 +3815,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E49" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J49,J49)</f>
@@ -3831,10 +3840,10 @@
         <v>0.01824</v>
       </c>
       <c r="J49" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="K49" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3845,10 +3854,10 @@
         <v>2</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E50" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J50,J50)</f>
@@ -3870,10 +3879,10 @@
         <v>0.012</v>
       </c>
       <c r="J50" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,10 +3893,10 @@
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E51" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J51,J51)</f>
@@ -3909,32 +3918,32 @@
         <v>0.02448</v>
       </c>
       <c r="J51" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="K51" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>120</v>
+        <v>220</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E52" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J52,J52)</f>
-        <v>311-120GRCT-ND</v>
+        <v>311-220GRCT-ND</v>
       </c>
       <c r="F52" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K52,K52)</f>
-        <v>71-CRCW0603-120-E3</v>
+        <v>71-CRCW0603-220-E3</v>
       </c>
       <c r="G52" s="2" t="n">
         <f aca="false">100*B52</f>
@@ -3948,24 +3957,24 @@
         <v>0.0045</v>
       </c>
       <c r="J52" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K52" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E53" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J53,J53)</f>
@@ -3987,10 +3996,10 @@
         <v>0.44</v>
       </c>
       <c r="J53" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4001,10 +4010,10 @@
         <v>4</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E54" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J54,J54)</f>
@@ -4026,10 +4035,10 @@
         <v>0.01392</v>
       </c>
       <c r="J54" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K54" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,10 +4049,10 @@
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E55" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J55,J55)</f>
@@ -4065,32 +4074,32 @@
         <v>0.02224</v>
       </c>
       <c r="J55" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K55" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K55" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>680</v>
+        <v>390</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E56" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J56,J56)</f>
-        <v>311-680GRCT-ND</v>
+        <v>311-390GRCT-ND</v>
       </c>
       <c r="F56" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K56,K56)</f>
-        <v>71-CRCW0603-680-E3</v>
+        <v>71-CRCW0603-390-E3</v>
       </c>
       <c r="G56" s="2" t="n">
         <f aca="false">100*B56</f>
@@ -4104,24 +4113,24 @@
         <v>0.009</v>
       </c>
       <c r="J56" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="K56" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E57" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J57,J57)</f>
@@ -4143,24 +4152,24 @@
         <v>0.009</v>
       </c>
       <c r="J57" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K57" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E58" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J58,J58)</f>
@@ -4182,24 +4191,24 @@
         <v>0.01044</v>
       </c>
       <c r="J58" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K58" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E59" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J59,J59)</f>
@@ -4221,24 +4230,24 @@
         <v>0.01392</v>
       </c>
       <c r="J59" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K59" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E60" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J60,J60)</f>
@@ -4260,24 +4269,24 @@
         <v>0.1434</v>
       </c>
       <c r="J60" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K60" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>5</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E61" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J61,J61)</f>
@@ -4299,24 +4308,24 @@
         <v>0.0139</v>
       </c>
       <c r="J61" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="K61" s="2" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B62" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E62" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J62,J62)</f>
@@ -4328,34 +4337,34 @@
       </c>
       <c r="G62" s="2" t="n">
         <f aca="false">100*B62</f>
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="H62" s="9" t="n">
         <v>0.00177</v>
       </c>
       <c r="I62" s="9" t="n">
         <f aca="false">B62*H62</f>
-        <v>0.04425</v>
+        <v>0.04071</v>
       </c>
       <c r="J62" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K62" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B63" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E63" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J63,J63)</f>
@@ -4377,24 +4386,24 @@
         <v>0.01368</v>
       </c>
       <c r="J63" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>15</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E64" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J64,J64)</f>
@@ -4416,24 +4425,24 @@
         <v>1.11915</v>
       </c>
       <c r="J64" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="K64" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E65" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J65,J65)</f>
@@ -4455,24 +4464,24 @@
         <v>0.1434</v>
       </c>
       <c r="J65" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K65" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="K65" s="2" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B66" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="D66" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E66" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J66,J66)</f>
@@ -4484,34 +4493,34 @@
       </c>
       <c r="G66" s="2" t="n">
         <f aca="false">100*B66</f>
-        <v>1100</v>
+        <v>1300</v>
       </c>
       <c r="H66" s="9" t="n">
         <v>0.00204</v>
       </c>
       <c r="I66" s="9" t="n">
         <f aca="false">B66*H66</f>
-        <v>0.02244</v>
+        <v>0.02652</v>
       </c>
       <c r="J66" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K66" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E67" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J67,J67)</f>
@@ -4533,24 +4542,24 @@
         <v>0.0045</v>
       </c>
       <c r="J67" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="K67" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="E68" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J68,J68)</f>
@@ -4572,24 +4581,24 @@
         <v>0.1378</v>
       </c>
       <c r="J68" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="K68" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="E69" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J69,J69)</f>
@@ -4611,32 +4620,32 @@
         <v>0.1582</v>
       </c>
       <c r="J69" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="K69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K69" s="2" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>302</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E70" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J70,J70)</f>
-        <v>NSI45020T1GOSCT-ND</v>
+        <v>NSI50010YT1GOSCT-ND</v>
       </c>
       <c r="F70" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K70,K70)</f>
-        <v>863-NSI45020AT1G</v>
+        <v>863-NSI50010YT1G</v>
       </c>
       <c r="G70" s="2" t="n">
         <f aca="false">100*B70</f>
@@ -4650,24 +4659,24 @@
         <v>1.7094</v>
       </c>
       <c r="J70" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="K70" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="E71" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J71,J71)</f>
@@ -4689,24 +4698,24 @@
         <v>0.2264</v>
       </c>
       <c r="J71" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K71" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="E72" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J72,J72)</f>
@@ -4728,24 +4737,24 @@
         <v>0.4158</v>
       </c>
       <c r="J72" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K72" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B73" s="2" t="n">
         <v>7</v>
       </c>
       <c r="C73" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="E73" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J73,J73)</f>
@@ -4767,24 +4776,24 @@
         <v>1.176</v>
       </c>
       <c r="J73" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K73" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B74" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="E74" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J74,J74)</f>
@@ -4806,24 +4815,24 @@
         <v>0.2426</v>
       </c>
       <c r="J74" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="K74" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="E75" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J75,J75)</f>
@@ -4845,24 +4854,24 @@
         <v>0.89772</v>
       </c>
       <c r="J75" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="K75" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C76" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="E76" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J76,J76)</f>
@@ -4884,24 +4893,24 @@
         <v>0.76</v>
       </c>
       <c r="J76" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K76" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="E77" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J77,J77)</f>
@@ -4923,24 +4932,24 @@
         <v>0.7182</v>
       </c>
       <c r="J77" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="K77" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>345</v>
       </c>
       <c r="E78" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J78,J78)</f>
@@ -4962,24 +4971,24 @@
         <v>0.9233</v>
       </c>
       <c r="J78" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="K78" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C79" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="E79" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J79,J79)</f>
@@ -5001,24 +5010,24 @@
         <v>0.2537</v>
       </c>
       <c r="J79" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="K79" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B80" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C80" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>355</v>
       </c>
       <c r="E80" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J80,J80)</f>
@@ -5040,24 +5049,24 @@
         <v>0.7671</v>
       </c>
       <c r="J80" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="K80" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C81" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="E81" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J81,J81)</f>
@@ -5079,24 +5088,24 @@
         <v>1.44</v>
       </c>
       <c r="J81" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="K81" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B82" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="E82" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J82,J82)</f>
@@ -5118,24 +5127,24 @@
         <v>2.675</v>
       </c>
       <c r="J82" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="K82" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B83" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C83" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="E83" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J83,J83)</f>
@@ -5157,24 +5166,24 @@
         <v>0.2652</v>
       </c>
       <c r="J83" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K83" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C84" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="E84" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J84,J84)</f>
@@ -5196,24 +5205,24 @@
         <v>1.6704</v>
       </c>
       <c r="J84" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="K84" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B85" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="E85" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J85,J85)</f>
@@ -5235,24 +5244,24 @@
         <v>2.412</v>
       </c>
       <c r="J85" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="K85" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B86" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="E86" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J86,J86)</f>
@@ -5274,24 +5283,24 @@
         <v>5.4</v>
       </c>
       <c r="J86" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K86" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="E87" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J87,J87)</f>
@@ -5313,24 +5322,24 @@
         <v>0.2605</v>
       </c>
       <c r="J87" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K87" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C88" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="E88" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J88,J88)</f>
@@ -5352,24 +5361,24 @@
         <v>0.2086</v>
       </c>
       <c r="J88" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="K88" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B89" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C89" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="E89" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J89,J89)</f>
@@ -5391,24 +5400,24 @@
         <v>3.1017</v>
       </c>
       <c r="J89" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="K89" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C90" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="E90" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J90,J90)</f>
@@ -5430,24 +5439,24 @@
         <v>1.0017</v>
       </c>
       <c r="J90" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="K90" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B91" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C91" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="E91" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J91,J91)</f>
@@ -5469,24 +5478,24 @@
         <v>3.4182</v>
       </c>
       <c r="J91" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="K91" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B92" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="E92" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J92,J92)</f>
@@ -5508,24 +5517,24 @@
         <v>0.3127</v>
       </c>
       <c r="J92" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="K92" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B93" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C93" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="E93" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J93,J93)</f>
@@ -5547,24 +5556,24 @@
         <v>0.3578</v>
       </c>
       <c r="J93" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="K93" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C94" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="E94" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J94,J94)</f>
@@ -5586,24 +5595,24 @@
         <v>11.05</v>
       </c>
       <c r="J94" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="K94" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B95" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C95" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="E95" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J95,J95)</f>
@@ -5625,24 +5634,24 @@
         <v>0.4985</v>
       </c>
       <c r="J95" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="K95" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C96" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="E96" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J96,J96)</f>
@@ -5664,24 +5673,24 @@
         <v>0.432</v>
       </c>
       <c r="J96" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="K96" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="K96" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E97" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J97,J97)</f>
@@ -5703,24 +5712,24 @@
         <v>1.6</v>
       </c>
       <c r="J97" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="K97" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B98" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C98" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="E98" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J98,J98)</f>
@@ -5742,24 +5751,24 @@
         <v>0.99872</v>
       </c>
       <c r="J98" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K98" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B99" s="2" t="n">
         <v>9</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E99" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J99,J99)</f>
@@ -5781,24 +5790,24 @@
         <v>2.06928</v>
       </c>
       <c r="J99" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="K99" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C100" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="E100" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J100,J100)</f>
@@ -5820,126 +5829,126 @@
         <v>0.1247</v>
       </c>
       <c r="J100" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="K100" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="101" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F101" s="0"/>
-      <c r="G101" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="H101" s="10"/>
+      <c r="G101" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="H101" s="11"/>
       <c r="I101" s="9" t="n">
         <f aca="false">SUM(I2:I100)</f>
-        <v>94.34056</v>
+        <v>94.2963</v>
       </c>
     </row>
     <row r="102" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="11"/>
+      <c r="J102" s="12"/>
     </row>
     <row r="103" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F103" s="12"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12" t="s">
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="I103" s="14" t="n">
+        <v>40</v>
+      </c>
+      <c r="J103" s="12"/>
+    </row>
+    <row r="104" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F104" s="13"/>
+      <c r="G104" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="I103" s="13" t="n">
-        <v>40</v>
-      </c>
-      <c r="J103" s="11"/>
-    </row>
-    <row r="104" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F104" s="12"/>
-      <c r="G104" s="14" t="s">
+      <c r="H104" s="15"/>
+      <c r="I104" s="16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J104" s="12"/>
+    </row>
+    <row r="105" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="13"/>
+      <c r="H105" s="17" t="s">
         <v>458</v>
-      </c>
-      <c r="H104" s="14"/>
-      <c r="I104" s="15" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J104" s="11"/>
-    </row>
-    <row r="105" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G105" s="12"/>
-      <c r="H105" s="16" t="s">
-        <v>459</v>
       </c>
       <c r="I105" s="9" t="n">
         <f aca="false">I104*(I101+I103/100)</f>
-        <v>28.422168</v>
-      </c>
-      <c r="J105" s="11"/>
+        <v>28.40889</v>
+      </c>
+      <c r="J105" s="12"/>
     </row>
     <row r="106" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="107" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H107" s="12" t="s">
+      <c r="H107" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="I107" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="I107" s="17" t="s">
+      <c r="J107" s="19"/>
+      <c r="L107" s="20"/>
+    </row>
+    <row r="108" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H108" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="J107" s="18"/>
-      <c r="L107" s="19"/>
-    </row>
-    <row r="108" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H108" s="12" t="s">
+      <c r="I108" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="J108" s="19"/>
+      <c r="L108" s="20"/>
+    </row>
+    <row r="109" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H109" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="I108" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="J108" s="18"/>
-      <c r="L108" s="19"/>
-    </row>
-    <row r="109" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H109" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="I109" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="J109" s="18"/>
-      <c r="L109" s="19"/>
+      <c r="I109" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="J109" s="19"/>
+      <c r="L109" s="20"/>
     </row>
     <row r="110" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="111" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F111" s="20" t="s">
-        <v>464</v>
-      </c>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="21" t="n">
+      <c r="F111" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="22" t="n">
         <f aca="false">SUM(I107:I109,I101,I105,I103/100)</f>
-        <v>123.162728</v>
-      </c>
-      <c r="J111" s="22"/>
+        <v>123.10519</v>
+      </c>
+      <c r="J111" s="23"/>
     </row>
     <row r="112" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="23" t="s">
-        <v>465</v>
-      </c>
-      <c r="B113" s="23"/>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="23"/>
-      <c r="H113" s="23"/>
-      <c r="I113" s="23"/>
+      <c r="A113" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+      <c r="I113" s="24"/>
     </row>
     <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B114" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E114" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J114,J114)</f>
@@ -5961,21 +5970,21 @@
         <v>12.14496</v>
       </c>
       <c r="J114" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K114" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B115" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E115" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J115,J115)</f>
@@ -5997,21 +6006,21 @@
         <v>2.394</v>
       </c>
       <c r="J115" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="K115" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B116" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E116" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J116,J116)</f>
@@ -6033,21 +6042,21 @@
         <v>7.4696</v>
       </c>
       <c r="J116" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="K116" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B117" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E117" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J117,J117)</f>
@@ -6069,10 +6078,10 @@
         <v>1.588</v>
       </c>
       <c r="J117" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="K117" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6080,21 +6089,21 @@
       <c r="I118" s="2"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F119" s="24" t="s">
-        <v>456</v>
-      </c>
-      <c r="G119" s="24"/>
-      <c r="H119" s="24"/>
+      <c r="F119" s="25" t="s">
+        <v>455</v>
+      </c>
+      <c r="G119" s="25"/>
+      <c r="H119" s="25"/>
       <c r="I119" s="9" t="n">
         <f aca="false">SUM(I2:I29,I32:I100,I114:I117)</f>
-        <v>114.14212</v>
+        <v>114.09786</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G120" s="16" t="s">
-        <v>482</v>
-      </c>
-      <c r="H120" s="16"/>
+      <c r="G120" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="H120" s="17"/>
       <c r="I120" s="9" t="n">
         <f aca="false">I119-I101</f>
         <v>19.80156</v>
@@ -6105,12 +6114,12 @@
       <c r="I121" s="2"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H122" s="16" t="s">
-        <v>459</v>
+      <c r="H122" s="17" t="s">
+        <v>458</v>
       </c>
       <c r="I122" s="9" t="n">
         <f aca="false">I104*(I119+I103/100)</f>
-        <v>34.362636</v>
+        <v>34.349358</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6118,14 +6127,14 @@
       <c r="I123" s="2"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F124" s="20" t="s">
-        <v>464</v>
-      </c>
-      <c r="G124" s="20"/>
-      <c r="H124" s="20"/>
-      <c r="I124" s="21" t="n">
+      <c r="F124" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="G124" s="21"/>
+      <c r="H124" s="21"/>
+      <c r="I124" s="22" t="n">
         <f aca="false">SUM(I107:I109,I119,I122,I103/100)</f>
-        <v>148.904756</v>
+        <v>148.847218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resistors added on open drain outputs.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -11,16 +11,16 @@
     <sheet name="ciaa-nxp" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ciaa-nxp'!$A$1:$C$100</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="ciaa_nxp_1" vbProcedure="false">'ciaa-nxp'!$A$2:$C$100</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ciaa-nxp'!$A$1:$C$100</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ciaa-nxp'!$A$1:$C$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="ciaa_nxp_1" vbProcedure="false">'ciaa-nxp'!$A$2:$C$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ciaa-nxp'!$A$1:$C$101</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="487">
   <si>
     <t>Componente</t>
   </si>
@@ -776,6 +776,21 @@
   </si>
   <si>
     <t>71-CRCW0603-1.0K-E3</t>
+  </si>
+  <si>
+    <t>1k5 250mW</t>
+  </si>
+  <si>
+    <t>R31 R81 R113 R139</t>
+  </si>
+  <si>
+    <t>Resistor SMD 1206</t>
+  </si>
+  <si>
+    <t>CR1206-JW-152ELFCT-ND</t>
+  </si>
+  <si>
+    <t>652-CR1206JW-152ELF</t>
   </si>
   <si>
     <t>1k5</t>
@@ -1868,15 +1883,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>615240</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:colOff>616680</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1541160</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1885,8 +1900,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8132760" y="20530440"/>
-          <a:ext cx="2531880" cy="1508040"/>
+          <a:off x="8134200" y="20710800"/>
+          <a:ext cx="2530440" cy="1389240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1929,10 +1944,10 @@
     <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4119,7 +4134,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>248</v>
       </c>
@@ -4158,427 +4173,427 @@
         <v>251</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>253</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>210</v>
+        <v>254</v>
       </c>
       <c r="E58" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J58,J58)</f>
-        <v>311-1.5KGRCT-ND</v>
+        <v>CR1206-JW-152ELFCT-ND</v>
       </c>
       <c r="F58" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K58,K58)</f>
-        <v>71-CRCW0603-1.5K-E3</v>
+        <v>652-CR1206JW-152ELF</v>
       </c>
       <c r="G58" s="2" t="n">
         <f aca="false">100*B58</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H58" s="9" t="n">
-        <v>0.00348</v>
+        <v>0.1</v>
       </c>
       <c r="I58" s="9" t="n">
         <f aca="false">B58*H58</f>
-        <v>0.01044</v>
+        <v>0.4</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E59" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J59,J59)</f>
-        <v>311-2.2KGRCT-ND</v>
+        <v>311-1.5KGRCT-ND</v>
       </c>
       <c r="F59" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K59,K59)</f>
-        <v>71-CRCW0603-2.2K-E3</v>
+        <v>71-CRCW0603-1.5K-E3</v>
       </c>
       <c r="G59" s="2" t="n">
         <f aca="false">100*B59</f>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H59" s="9" t="n">
         <v>0.00348</v>
       </c>
       <c r="I59" s="9" t="n">
         <f aca="false">B59*H59</f>
-        <v>0.01392</v>
+        <v>0.01044</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E60" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J60,J60)</f>
-        <v>P2.49KDBCT-ND</v>
+        <v>311-2.2KGRCT-ND</v>
       </c>
       <c r="F60" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K60,K60)</f>
-        <v>756-PCF0603R-2K49BT1</v>
+        <v>71-CRCW0603-2.2K-E3</v>
       </c>
       <c r="G60" s="2" t="n">
         <f aca="false">100*B60</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="H60" s="9" t="n">
-        <v>0.1434</v>
+        <v>0.00348</v>
       </c>
       <c r="I60" s="9" t="n">
         <f aca="false">B60*H60</f>
-        <v>0.1434</v>
+        <v>0.01392</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E61" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J61,J61)</f>
-        <v>311-4.7KGRCT-ND</v>
+        <v>P2.49KDBCT-ND</v>
       </c>
       <c r="F61" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K61,K61)</f>
-        <v>71-CRCW0603-4.7K-E3</v>
+        <v>756-PCF0603R-2K49BT1</v>
       </c>
       <c r="G61" s="2" t="n">
         <f aca="false">100*B61</f>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="H61" s="9" t="n">
-        <v>0.00278</v>
+        <v>0.1434</v>
       </c>
       <c r="I61" s="9" t="n">
         <f aca="false">B61*H61</f>
-        <v>0.0139</v>
+        <v>0.1434</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E62" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J62,J62)</f>
-        <v>311-10KGRCT-ND</v>
+        <v>311-4.7KGRCT-ND</v>
       </c>
       <c r="F62" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K62,K62)</f>
-        <v>71-CRCW0603-10K-E3</v>
+        <v>71-CRCW0603-4.7K-E3</v>
       </c>
       <c r="G62" s="2" t="n">
         <f aca="false">100*B62</f>
-        <v>2300</v>
+        <v>500</v>
       </c>
       <c r="H62" s="9" t="n">
-        <v>0.00177</v>
+        <v>0.00278</v>
       </c>
       <c r="I62" s="9" t="n">
         <f aca="false">B62*H62</f>
-        <v>0.04071</v>
+        <v>0.0139</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E63" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J63,J63)</f>
-        <v>311-12.1KHRCT-ND</v>
+        <v>311-10KGRCT-ND</v>
       </c>
       <c r="F63" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K63,K63)</f>
-        <v>71-CRCW0603-12.1K-E3</v>
+        <v>71-CRCW0603-10K-E3</v>
       </c>
       <c r="G63" s="2" t="n">
         <f aca="false">100*B63</f>
-        <v>300</v>
+        <v>2300</v>
       </c>
       <c r="H63" s="9" t="n">
-        <v>0.00456</v>
+        <v>0.00177</v>
       </c>
       <c r="I63" s="9" t="n">
         <f aca="false">B63*H63</f>
-        <v>0.01368</v>
+        <v>0.04071</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E64" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J64,J64)</f>
-        <v>RG16P15.0KBCT-ND</v>
+        <v>311-12.1KHRCT-ND</v>
       </c>
       <c r="F64" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K64,K64)</f>
-        <v>756-PCF0603R-15KBT1</v>
+        <v>71-CRCW0603-12.1K-E3</v>
       </c>
       <c r="G64" s="2" t="n">
         <f aca="false">100*B64</f>
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="H64" s="9" t="n">
-        <v>0.07461</v>
+        <v>0.00456</v>
       </c>
       <c r="I64" s="9" t="n">
         <f aca="false">B64*H64</f>
-        <v>1.11915</v>
+        <v>0.01368</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E65" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J65,J65)</f>
-        <v>P33KDBCT-ND</v>
+        <v>RG16P15.0KBCT-ND</v>
       </c>
       <c r="F65" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K65,K65)</f>
-        <v>754-RG1608P-333-BT5</v>
+        <v>756-PCF0603R-15KBT1</v>
       </c>
       <c r="G65" s="2" t="n">
         <f aca="false">100*B65</f>
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="H65" s="9" t="n">
-        <v>0.1434</v>
+        <v>0.07461</v>
       </c>
       <c r="I65" s="9" t="n">
         <f aca="false">B65*H65</f>
-        <v>0.1434</v>
+        <v>1.11915</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E66" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J66,J66)</f>
-        <v>311-100KGRCT-ND</v>
+        <v>P33KDBCT-ND</v>
       </c>
       <c r="F66" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K66,K66)</f>
-        <v>71-CRCW0603-100K-E3</v>
+        <v>754-RG1608P-333-BT5</v>
       </c>
       <c r="G66" s="2" t="n">
         <f aca="false">100*B66</f>
-        <v>1300</v>
+        <v>100</v>
       </c>
       <c r="H66" s="9" t="n">
-        <v>0.00204</v>
+        <v>0.1434</v>
       </c>
       <c r="I66" s="9" t="n">
         <f aca="false">B66*H66</f>
-        <v>0.02652</v>
+        <v>0.1434</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E67" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J67,J67)</f>
-        <v>311-10MGRCT-ND</v>
+        <v>311-100KGRCT-ND</v>
       </c>
       <c r="F67" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K67,K67)</f>
-        <v>71-CRCW0603-10M-E3</v>
+        <v>71-CRCW0603-100K-E3</v>
       </c>
       <c r="G67" s="2" t="n">
         <f aca="false">100*B67</f>
-        <v>100</v>
+        <v>1300</v>
       </c>
       <c r="H67" s="9" t="n">
-        <v>0.0045</v>
+        <v>0.00204</v>
       </c>
       <c r="I67" s="9" t="n">
         <f aca="false">B67*H67</f>
-        <v>0.0045</v>
+        <v>0.02652</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>294</v>
+        <v>210</v>
       </c>
       <c r="E68" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J68,J68)</f>
-        <v>CR2010-JW-101ELFCT-ND</v>
+        <v>311-10MGRCT-ND</v>
       </c>
       <c r="F68" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K68,K68)</f>
-        <v>660-SG73P2ETTD1000F</v>
+        <v>71-CRCW0603-10M-E3</v>
       </c>
       <c r="G68" s="2" t="n">
         <f aca="false">100*B68</f>
         <v>100</v>
       </c>
       <c r="H68" s="9" t="n">
-        <v>0.1378</v>
+        <v>0.0045</v>
       </c>
       <c r="I68" s="9" t="n">
         <f aca="false">B68*H68</f>
-        <v>0.1378</v>
+        <v>0.0045</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>295</v>
@@ -4602,22 +4617,22 @@
       </c>
       <c r="E69" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J69,J69)</f>
-        <v>450-1792-1-ND</v>
+        <v>CR2010-JW-101ELFCT-ND</v>
       </c>
       <c r="F69" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K69,K69)</f>
-        <v>612-TL3301BF260QG</v>
+        <v>660-SG73P2ETTD1000F</v>
       </c>
       <c r="G69" s="2" t="n">
         <f aca="false">100*B69</f>
         <v>100</v>
       </c>
       <c r="H69" s="9" t="n">
-        <v>0.1582</v>
+        <v>0.1378</v>
       </c>
       <c r="I69" s="9" t="n">
         <f aca="false">B69*H69</f>
-        <v>0.1582</v>
+        <v>0.1378</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>300</v>
@@ -4626,12 +4641,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>302</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>303</v>
@@ -4641,22 +4656,22 @@
       </c>
       <c r="E70" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J70,J70)</f>
-        <v>NSI50010YT1GOSCT-ND</v>
+        <v>450-1792-1-ND</v>
       </c>
       <c r="F70" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K70,K70)</f>
-        <v>863-NSI50010YT1G</v>
+        <v>612-TL3301BF260QG</v>
       </c>
       <c r="G70" s="2" t="n">
         <f aca="false">100*B70</f>
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="H70" s="9" t="n">
-        <v>0.14245</v>
+        <v>0.1582</v>
       </c>
       <c r="I70" s="9" t="n">
         <f aca="false">B70*H70</f>
-        <v>1.7094</v>
+        <v>0.1582</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>305</v>
@@ -4665,37 +4680,37 @@
         <v>306</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>307</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>309</v>
       </c>
       <c r="E71" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J71,J71)</f>
-        <v>MF-USMF005-2CT-ND</v>
+        <v>NSI50010YT1GOSCT-ND</v>
       </c>
       <c r="F71" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K71,K71)</f>
-        <v>652-MF-USMF005-2</v>
+        <v>863-NSI50010YT1G</v>
       </c>
       <c r="G71" s="2" t="n">
         <f aca="false">100*B71</f>
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="H71" s="9" t="n">
-        <v>0.2264</v>
+        <v>0.14245</v>
       </c>
       <c r="I71" s="9" t="n">
         <f aca="false">B71*H71</f>
-        <v>0.2264</v>
+        <v>1.7094</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>310</v>
@@ -4714,27 +4729,27 @@
       <c r="C72" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="3" t="s">
         <v>314</v>
       </c>
       <c r="E72" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J72,J72)</f>
-        <v>MF-SM300-2CT-ND</v>
+        <v>MF-USMF005-2CT-ND</v>
       </c>
       <c r="F72" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K72,K72)</f>
-        <v>504-PTS18126V300</v>
+        <v>652-MF-USMF005-2</v>
       </c>
       <c r="G72" s="2" t="n">
         <f aca="false">100*B72</f>
         <v>100</v>
       </c>
       <c r="H72" s="9" t="n">
-        <v>0.4158</v>
+        <v>0.2264</v>
       </c>
       <c r="I72" s="9" t="n">
         <f aca="false">B72*H72</f>
-        <v>0.4158</v>
+        <v>0.2264</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>315</v>
@@ -4748,7 +4763,7 @@
         <v>317</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>318</v>
@@ -4758,22 +4773,22 @@
       </c>
       <c r="E73" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J73,J73)</f>
-        <v>MF-USMF110-2CT-ND</v>
+        <v>MF-SM300-2CT-ND</v>
       </c>
       <c r="F73" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K73,K73)</f>
-        <v>504-PTS12066V100</v>
+        <v>504-PTS18126V300</v>
       </c>
       <c r="G73" s="2" t="n">
         <f aca="false">100*B73</f>
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="H73" s="9" t="n">
-        <v>0.168</v>
+        <v>0.4158</v>
       </c>
       <c r="I73" s="9" t="n">
         <f aca="false">B73*H73</f>
-        <v>1.176</v>
+        <v>0.4158</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>320</v>
@@ -4787,7 +4802,7 @@
         <v>322</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>323</v>
@@ -4797,22 +4812,22 @@
       </c>
       <c r="E74" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J74,J74)</f>
-        <v>MF-MSMF030-2CT-ND</v>
+        <v>MF-USMF110-2CT-ND</v>
       </c>
       <c r="F74" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K74,K74)</f>
-        <v>652-MF-MSMF030-2</v>
+        <v>504-PTS12066V100</v>
       </c>
       <c r="G74" s="2" t="n">
         <f aca="false">100*B74</f>
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="H74" s="9" t="n">
-        <v>0.2426</v>
+        <v>0.168</v>
       </c>
       <c r="I74" s="9" t="n">
         <f aca="false">B74*H74</f>
-        <v>0.2426</v>
+        <v>1.176</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>325</v>
@@ -4826,7 +4841,7 @@
         <v>327</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>328</v>
@@ -4836,22 +4851,22 @@
       </c>
       <c r="E75" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J75,J75)</f>
-        <v>SRF2012-900YCT-ND</v>
+        <v>MF-MSMF030-2CT-ND</v>
       </c>
       <c r="F75" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K75,K75)</f>
-        <v>81-DLW21HN900SQ2L</v>
+        <v>652-MF-MSMF030-2</v>
       </c>
       <c r="G75" s="2" t="n">
         <f aca="false">100*B75</f>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="H75" s="9" t="n">
-        <v>0.29924</v>
+        <v>0.2426</v>
       </c>
       <c r="I75" s="9" t="n">
         <f aca="false">B75*H75</f>
-        <v>0.89772</v>
+        <v>0.2426</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>330</v>
@@ -4865,7 +4880,7 @@
         <v>332</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>333</v>
@@ -4875,22 +4890,22 @@
       </c>
       <c r="E76" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J76,J76)</f>
-        <v>LAN8720A-CP-CT-ND</v>
+        <v>SRF2012-900YCT-ND</v>
       </c>
       <c r="F76" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K76,K76)</f>
-        <v>886-LAN8720A-CP-TR</v>
+        <v>81-DLW21HN900SQ2L</v>
       </c>
       <c r="G76" s="2" t="n">
         <f aca="false">100*B76</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H76" s="9" t="n">
-        <v>0.76</v>
+        <v>0.29924</v>
       </c>
       <c r="I76" s="9" t="n">
         <f aca="false">B76*H76</f>
-        <v>0.76</v>
+        <v>0.89772</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>335</v>
@@ -4914,22 +4929,22 @@
       </c>
       <c r="E77" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J77,J77)</f>
-        <v>497-6538-1-ND</v>
+        <v>LAN8720A-CP-CT-ND</v>
       </c>
       <c r="F77" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K77,K77)</f>
-        <v>511-ST3232EC</v>
+        <v>886-LAN8720A-CP-TR</v>
       </c>
       <c r="G77" s="2" t="n">
         <f aca="false">100*B77</f>
         <v>100</v>
       </c>
       <c r="H77" s="9" t="n">
-        <v>0.7182</v>
+        <v>0.76</v>
       </c>
       <c r="I77" s="9" t="n">
         <f aca="false">B77*H77</f>
-        <v>0.7182</v>
+        <v>0.76</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>340</v>
@@ -4953,22 +4968,22 @@
       </c>
       <c r="E78" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J78,J78)</f>
-        <v>568-10289-1-ND</v>
+        <v>497-6538-1-ND</v>
       </c>
       <c r="F78" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K78,K78)</f>
-        <v>579-MCP2561-E/SN</v>
+        <v>511-ST3232EC</v>
       </c>
       <c r="G78" s="2" t="n">
         <f aca="false">100*B78</f>
         <v>100</v>
       </c>
       <c r="H78" s="9" t="n">
-        <v>0.9233</v>
+        <v>0.7182</v>
       </c>
       <c r="I78" s="9" t="n">
         <f aca="false">B78*H78</f>
-        <v>0.9233</v>
+        <v>0.7182</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>345</v>
@@ -4992,22 +5007,22 @@
       </c>
       <c r="E79" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J79,J79)</f>
-        <v>568-4032-1-ND</v>
+        <v>568-10289-1-ND</v>
       </c>
       <c r="F79" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K79,K79)</f>
-        <v>771-PESD1CAN-T/R</v>
+        <v>579-MCP2561-E/SN</v>
       </c>
       <c r="G79" s="2" t="n">
         <f aca="false">100*B79</f>
         <v>100</v>
       </c>
       <c r="H79" s="9" t="n">
-        <v>0.2537</v>
+        <v>0.9233</v>
       </c>
       <c r="I79" s="9" t="n">
         <f aca="false">B79*H79</f>
-        <v>0.2537</v>
+        <v>0.9233</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>350</v>
@@ -5031,22 +5046,22 @@
       </c>
       <c r="E80" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J80,J80)</f>
-        <v>576-1058-ND</v>
+        <v>568-4032-1-ND</v>
       </c>
       <c r="F80" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K80,K80)</f>
-        <v>998-MIC2025-2YMTR</v>
+        <v>771-PESD1CAN-T/R</v>
       </c>
       <c r="G80" s="2" t="n">
         <f aca="false">100*B80</f>
         <v>100</v>
       </c>
       <c r="H80" s="9" t="n">
-        <v>0.7671</v>
+        <v>0.2537</v>
       </c>
       <c r="I80" s="9" t="n">
         <f aca="false">B80*H80</f>
-        <v>0.7671</v>
+        <v>0.2537</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>355</v>
@@ -5070,22 +5085,22 @@
       </c>
       <c r="E81" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J81,J81)</f>
-        <v>MCP6024-I/ST-ND</v>
+        <v>576-1058-ND</v>
       </c>
       <c r="F81" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K81,K81)</f>
-        <v>579-MCP6024-I/ST</v>
+        <v>998-MIC2025-2YMTR</v>
       </c>
       <c r="G81" s="2" t="n">
         <f aca="false">100*B81</f>
         <v>100</v>
       </c>
       <c r="H81" s="9" t="n">
-        <v>1.44</v>
+        <v>0.7671</v>
       </c>
       <c r="I81" s="9" t="n">
         <f aca="false">B81*H81</f>
-        <v>1.44</v>
+        <v>0.7671</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>360</v>
@@ -5109,22 +5124,22 @@
       </c>
       <c r="E82" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J82,J82)</f>
-        <v>24AA1025-I/SN-ND</v>
+        <v>MCP6024-I/ST-ND</v>
       </c>
       <c r="F82" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K82,K82)</f>
-        <v>579-24AA1025T-I/SN</v>
+        <v>579-MCP6024-I/ST</v>
       </c>
       <c r="G82" s="2" t="n">
         <f aca="false">100*B82</f>
         <v>100</v>
       </c>
       <c r="H82" s="9" t="n">
-        <v>2.675</v>
+        <v>1.44</v>
       </c>
       <c r="I82" s="9" t="n">
         <f aca="false">B82*H82</f>
-        <v>2.675</v>
+        <v>1.44</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>365</v>
@@ -5148,22 +5163,22 @@
       </c>
       <c r="E83" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J83,J83)</f>
-        <v>24AA025E48-I/SN-ND</v>
+        <v>24AA1025-I/SN-ND</v>
       </c>
       <c r="F83" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K83,K83)</f>
-        <v>579-24AA025E48T-I/SN</v>
+        <v>579-24AA1025T-I/SN</v>
       </c>
       <c r="G83" s="2" t="n">
         <f aca="false">100*B83</f>
         <v>100</v>
       </c>
       <c r="H83" s="9" t="n">
-        <v>0.2652</v>
+        <v>2.675</v>
       </c>
       <c r="I83" s="9" t="n">
         <f aca="false">B83*H83</f>
-        <v>0.2652</v>
+        <v>2.675</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>370</v>
@@ -5187,22 +5202,22 @@
       </c>
       <c r="E84" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J84,J84)</f>
-        <v>296-21527-1-ND</v>
+        <v>24AA025E48-I/SN-ND</v>
       </c>
       <c r="F84" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K84,K84)</f>
-        <v>595-TXB0108PWR</v>
+        <v>579-24AA025E48T-I/SN</v>
       </c>
       <c r="G84" s="2" t="n">
         <f aca="false">100*B84</f>
         <v>100</v>
       </c>
       <c r="H84" s="9" t="n">
-        <v>1.6704</v>
+        <v>0.2652</v>
       </c>
       <c r="I84" s="9" t="n">
         <f aca="false">B84*H84</f>
-        <v>1.6704</v>
+        <v>0.2652</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>375</v>
@@ -5226,22 +5241,22 @@
       </c>
       <c r="E85" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J85,J85)</f>
-        <v>706-1077-ND</v>
+        <v>296-21527-1-ND</v>
       </c>
       <c r="F85" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K85,K85)</f>
-        <v>870-42S16400F-7TLI</v>
+        <v>595-TXB0108PWR</v>
       </c>
       <c r="G85" s="2" t="n">
         <f aca="false">100*B85</f>
         <v>100</v>
       </c>
       <c r="H85" s="9" t="n">
-        <v>2.412</v>
+        <v>1.6704</v>
       </c>
       <c r="I85" s="9" t="n">
         <f aca="false">B85*H85</f>
-        <v>2.412</v>
+        <v>1.6704</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>380</v>
@@ -5265,22 +5280,22 @@
       </c>
       <c r="E86" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J86,J86)</f>
-        <v>768-1024-1-ND</v>
+        <v>706-1077-ND</v>
       </c>
       <c r="F86" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K86,K86)</f>
-        <v>895-FT2232HL</v>
+        <v>870-42S16400F-7TLI</v>
       </c>
       <c r="G86" s="2" t="n">
         <f aca="false">100*B86</f>
         <v>100</v>
       </c>
       <c r="H86" s="9" t="n">
-        <v>5.4</v>
+        <v>2.412</v>
       </c>
       <c r="I86" s="9" t="n">
         <f aca="false">B86*H86</f>
-        <v>5.4</v>
+        <v>2.412</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>385</v>
@@ -5299,27 +5314,27 @@
       <c r="C87" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="2" t="s">
         <v>389</v>
       </c>
       <c r="E87" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J87,J87)</f>
-        <v>LM358DGOS-ND</v>
+        <v>768-1024-1-ND</v>
       </c>
       <c r="F87" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K87,K87)</f>
-        <v>863-LM358DG</v>
+        <v>895-FT2232HL</v>
       </c>
       <c r="G87" s="2" t="n">
         <f aca="false">100*B87</f>
         <v>100</v>
       </c>
       <c r="H87" s="9" t="n">
-        <v>0.2605</v>
+        <v>5.4</v>
       </c>
       <c r="I87" s="9" t="n">
         <f aca="false">B87*H87</f>
-        <v>0.2605</v>
+        <v>5.4</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>390</v>
@@ -5338,27 +5353,27 @@
       <c r="C88" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="3" t="s">
         <v>394</v>
       </c>
       <c r="E88" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J88,J88)</f>
-        <v>AT93C46DN-SH-B-ND</v>
+        <v>LM358DGOS-ND</v>
       </c>
       <c r="F88" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K88,K88)</f>
-        <v>579-93C46A-E/SN</v>
+        <v>863-LM358DG</v>
       </c>
       <c r="G88" s="2" t="n">
         <f aca="false">100*B88</f>
         <v>100</v>
       </c>
       <c r="H88" s="9" t="n">
-        <v>0.2086</v>
+        <v>0.2605</v>
       </c>
       <c r="I88" s="9" t="n">
         <f aca="false">B88*H88</f>
-        <v>0.2086</v>
+        <v>0.2605</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>395</v>
@@ -5382,22 +5397,22 @@
       </c>
       <c r="E89" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J89,J89)</f>
-        <v>296-26337-1-ND</v>
+        <v>AT93C46DN-SH-B-ND</v>
       </c>
       <c r="F89" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K89,K89)</f>
-        <v>595-SN65HVD1176DR</v>
+        <v>579-93C46A-E/SN</v>
       </c>
       <c r="G89" s="2" t="n">
         <f aca="false">100*B89</f>
         <v>100</v>
       </c>
       <c r="H89" s="9" t="n">
-        <v>3.1017</v>
+        <v>0.2086</v>
       </c>
       <c r="I89" s="9" t="n">
         <f aca="false">B89*H89</f>
-        <v>3.1017</v>
+        <v>0.2086</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>400</v>
@@ -5421,22 +5436,22 @@
       </c>
       <c r="E90" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J90,J90)</f>
-        <v>535-10829-1-ND</v>
+        <v>296-26337-1-ND</v>
       </c>
       <c r="F90" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K90,K90)</f>
-        <v>815-ASV-50.000M-E-T</v>
+        <v>595-SN65HVD1176DR</v>
       </c>
       <c r="G90" s="2" t="n">
         <f aca="false">100*B90</f>
         <v>100</v>
       </c>
       <c r="H90" s="9" t="n">
-        <v>1.0017</v>
+        <v>3.1017</v>
       </c>
       <c r="I90" s="9" t="n">
         <f aca="false">B90*H90</f>
-        <v>1.0017</v>
+        <v>3.1017</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>405</v>
@@ -5460,22 +5475,22 @@
       </c>
       <c r="E91" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J91,J91)</f>
-        <v>LM2596SX-5.0/NOPBCT-ND</v>
+        <v>535-10829-1-ND</v>
       </c>
       <c r="F91" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K91,K91)</f>
-        <v>926-LM2596SX-5.0NOPB</v>
+        <v>815-ASV-50.000M-E-T</v>
       </c>
       <c r="G91" s="2" t="n">
         <f aca="false">100*B91</f>
         <v>100</v>
       </c>
       <c r="H91" s="9" t="n">
-        <v>3.4182</v>
+        <v>1.0017</v>
       </c>
       <c r="I91" s="9" t="n">
         <f aca="false">B91*H91</f>
-        <v>3.4182</v>
+        <v>1.0017</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>410</v>
@@ -5499,22 +5514,22 @@
       </c>
       <c r="E92" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J92,J92)</f>
-        <v>NCP1117ST33T3GOSCT-ND</v>
+        <v>LM2596SX-5.0/NOPBCT-ND</v>
       </c>
       <c r="F92" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K92,K92)</f>
-        <v>863-NCP1117ST33T3G</v>
+        <v>926-LM2596SX-5.0NOPB</v>
       </c>
       <c r="G92" s="2" t="n">
         <f aca="false">100*B92</f>
         <v>100</v>
       </c>
       <c r="H92" s="9" t="n">
-        <v>0.3127</v>
+        <v>3.4182</v>
       </c>
       <c r="I92" s="9" t="n">
         <f aca="false">B92*H92</f>
-        <v>0.3127</v>
+        <v>3.4182</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>415</v>
@@ -5538,22 +5553,22 @@
       </c>
       <c r="E93" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J93,J93)</f>
-        <v>568-4140-1-ND</v>
+        <v>NCP1117ST33T3GOSCT-ND</v>
       </c>
       <c r="F93" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K93,K93)</f>
-        <v>771-PRTR5V0U2X-T/R</v>
+        <v>863-NCP1117ST33T3G</v>
       </c>
       <c r="G93" s="2" t="n">
         <f aca="false">100*B93</f>
         <v>100</v>
       </c>
       <c r="H93" s="9" t="n">
-        <v>0.3578</v>
+        <v>0.3127</v>
       </c>
       <c r="I93" s="9" t="n">
         <f aca="false">B93*H93</f>
-        <v>0.3578</v>
+        <v>0.3127</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>420</v>
@@ -5577,22 +5592,22 @@
       </c>
       <c r="E94" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J94,J94)</f>
-        <v>568-10159-ND</v>
+        <v>568-4140-1-ND</v>
       </c>
       <c r="F94" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K94,K94)</f>
-        <v>771-LPC4337JBD144E</v>
+        <v>771-PRTR5V0U2X-T/R</v>
       </c>
       <c r="G94" s="2" t="n">
         <f aca="false">100*B94</f>
         <v>100</v>
       </c>
       <c r="H94" s="9" t="n">
-        <v>11.05</v>
+        <v>0.3578</v>
       </c>
       <c r="I94" s="9" t="n">
         <f aca="false">B94*H94</f>
-        <v>11.05</v>
+        <v>0.3578</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>425</v>
@@ -5616,22 +5631,22 @@
       </c>
       <c r="E95" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J95,J95)</f>
-        <v>S25FL032P0XMFI011-ND</v>
+        <v>568-10159-ND</v>
       </c>
       <c r="F95" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K95,K95)</f>
-        <v>797-S25FL032P0XMFI01</v>
+        <v>771-LPC4337JBD144E</v>
       </c>
       <c r="G95" s="2" t="n">
         <f aca="false">100*B95</f>
         <v>100</v>
       </c>
       <c r="H95" s="9" t="n">
-        <v>0.4985</v>
+        <v>11.05</v>
       </c>
       <c r="I95" s="9" t="n">
         <f aca="false">B95*H95</f>
-        <v>0.4985</v>
+        <v>11.05</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>430</v>
@@ -5655,22 +5670,22 @@
       </c>
       <c r="E96" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J96,J96)</f>
-        <v>535-9166-1-ND</v>
+        <v>S25FL032P0XMFI011-ND</v>
       </c>
       <c r="F96" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K96,K96)</f>
-        <v>815-ABS25-32.768KHZT</v>
+        <v>797-S25FL032P0XMFI01</v>
       </c>
       <c r="G96" s="2" t="n">
         <f aca="false">100*B96</f>
         <v>100</v>
       </c>
       <c r="H96" s="9" t="n">
-        <v>0.432</v>
+        <v>0.4985</v>
       </c>
       <c r="I96" s="9" t="n">
         <f aca="false">B96*H96</f>
-        <v>0.432</v>
+        <v>0.4985</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>435</v>
@@ -5684,71 +5699,71 @@
         <v>437</v>
       </c>
       <c r="B97" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>438</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="E97" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J97,J97)</f>
-        <v>SER3683CT-ND</v>
+        <v>535-9166-1-ND</v>
       </c>
       <c r="F97" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K97,K97)</f>
-        <v>732-FA-238V12MB-W3</v>
+        <v>815-ABS25-32.768KHZT</v>
       </c>
       <c r="G97" s="2" t="n">
         <f aca="false">100*B97</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H97" s="9" t="n">
-        <v>0.8</v>
+        <v>0.432</v>
       </c>
       <c r="I97" s="9" t="n">
         <f aca="false">B97*H97</f>
-        <v>1.6</v>
+        <v>0.432</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B98" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E98" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J98,J98)</f>
-        <v>P6SMB20CAT3GOSCT-ND</v>
+        <v>SER3683CT-ND</v>
       </c>
       <c r="F98" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K98,K98)</f>
-        <v>576-P6SMB20CA</v>
+        <v>732-FA-238V12MB-W3</v>
       </c>
       <c r="G98" s="2" t="n">
         <f aca="false">100*B98</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H98" s="9" t="n">
-        <v>0.24968</v>
+        <v>0.8</v>
       </c>
       <c r="I98" s="9" t="n">
         <f aca="false">B98*H98</f>
-        <v>0.99872</v>
+        <v>1.6</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>444</v>
@@ -5762,71 +5777,71 @@
         <v>446</v>
       </c>
       <c r="B99" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>447</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="E99" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J99,J99)</f>
-        <v>P6SMB33CA-E3/52GICT-ND</v>
+        <v>P6SMB20CAT3GOSCT-ND</v>
       </c>
       <c r="F99" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K99,K99)</f>
-        <v>576-P6SMB33CA</v>
+        <v>576-P6SMB20CA</v>
       </c>
       <c r="G99" s="2" t="n">
         <f aca="false">100*B99</f>
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="H99" s="9" t="n">
-        <v>0.22992</v>
+        <v>0.24968</v>
       </c>
       <c r="I99" s="9" t="n">
         <f aca="false">B99*H99</f>
-        <v>2.06928</v>
+        <v>0.99872</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B100" s="2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E100" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J100,J100)</f>
-        <v>MMSZ5V6T1GOSCT-ND</v>
+        <v>P6SMB33CA-E3/52GICT-ND</v>
       </c>
       <c r="F100" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K100,K100)</f>
-        <v>78-BZT52C5V6-E3-08</v>
+        <v>576-P6SMB33CA</v>
       </c>
       <c r="G100" s="2" t="n">
         <f aca="false">100*B100</f>
-        <v>100</v>
+        <v>900</v>
       </c>
       <c r="H100" s="9" t="n">
-        <v>0.1247</v>
+        <v>0.22992</v>
       </c>
       <c r="I100" s="9" t="n">
         <f aca="false">B100*H100</f>
-        <v>0.1247</v>
+        <v>2.06928</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>453</v>
@@ -5835,317 +5850,356 @@
         <v>454</v>
       </c>
     </row>
-    <row r="101" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F101" s="0"/>
-      <c r="G101" s="11" t="s">
+    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="H101" s="11"/>
+      <c r="B101" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E101" s="8" t="str">
+        <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J101,J101)</f>
+        <v>MMSZ5V6T1GOSCT-ND</v>
+      </c>
+      <c r="F101" s="8" t="str">
+        <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K101,K101)</f>
+        <v>78-BZT52C5V6-E3-08</v>
+      </c>
+      <c r="G101" s="2" t="n">
+        <f aca="false">100*B101</f>
+        <v>100</v>
+      </c>
+      <c r="H101" s="9" t="n">
+        <v>0.1247</v>
+      </c>
       <c r="I101" s="9" t="n">
-        <f aca="false">SUM(I2:I100)</f>
-        <v>94.2963</v>
+        <f aca="false">B101*H101</f>
+        <v>0.1247</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="102" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="12"/>
+      <c r="F102" s="0"/>
+      <c r="G102" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="H102" s="11"/>
+      <c r="I102" s="9" t="n">
+        <f aca="false">SUM(I2:I101)</f>
+        <v>94.6963</v>
+      </c>
     </row>
     <row r="103" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13" t="s">
-        <v>456</v>
-      </c>
-      <c r="I103" s="14" t="n">
-        <v>40</v>
-      </c>
       <c r="J103" s="12"/>
     </row>
     <row r="104" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F104" s="13"/>
-      <c r="G104" s="15" t="s">
-        <v>457</v>
-      </c>
-      <c r="H104" s="15"/>
-      <c r="I104" s="16" t="n">
+      <c r="G104" s="13"/>
+      <c r="H104" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="I104" s="14" t="n">
+        <v>40</v>
+      </c>
+      <c r="J104" s="12"/>
+    </row>
+    <row r="105" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F105" s="13"/>
+      <c r="G105" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="H105" s="15"/>
+      <c r="I105" s="16" t="n">
         <v>0.3</v>
       </c>
-      <c r="J104" s="12"/>
-    </row>
-    <row r="105" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G105" s="13"/>
-      <c r="H105" s="17" t="s">
-        <v>458</v>
-      </c>
-      <c r="I105" s="9" t="n">
-        <f aca="false">I104*(I101+I103/100)</f>
-        <v>28.40889</v>
-      </c>
       <c r="J105" s="12"/>
     </row>
-    <row r="106" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H107" s="13" t="s">
-        <v>459</v>
-      </c>
-      <c r="I107" s="18" t="s">
-        <v>460</v>
-      </c>
-      <c r="J107" s="19"/>
-      <c r="L107" s="20"/>
-    </row>
+    <row r="106" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="13"/>
+      <c r="H106" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="I106" s="9" t="n">
+        <f aca="false">I105*(I102+I104/100)</f>
+        <v>28.52889</v>
+      </c>
+      <c r="J106" s="12"/>
+    </row>
+    <row r="107" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="108" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H108" s="13" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="I108" s="18" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="J108" s="19"/>
       <c r="L108" s="20"/>
     </row>
     <row r="109" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H109" s="13" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="I109" s="18" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="J109" s="19"/>
       <c r="L109" s="20"/>
     </row>
-    <row r="110" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F111" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="G111" s="21"/>
-      <c r="H111" s="21"/>
-      <c r="I111" s="22" t="n">
-        <f aca="false">SUM(I107:I109,I101,I105,I103/100)</f>
-        <v>123.10519</v>
-      </c>
-      <c r="J111" s="23"/>
-    </row>
-    <row r="112" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="24" t="s">
-        <v>464</v>
-      </c>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="24"/>
-      <c r="H113" s="24"/>
-      <c r="I113" s="24"/>
-    </row>
-    <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
+    <row r="110" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H110" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="I110" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="B114" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="E114" s="8" t="str">
-        <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J114,J114)</f>
-        <v>ED1723-ND</v>
-      </c>
-      <c r="F114" s="8" t="str">
-        <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K114,K114)</f>
-        <v>538-39530-0008</v>
-      </c>
-      <c r="G114" s="2" t="n">
-        <f aca="false">100*B114</f>
-        <v>400</v>
-      </c>
-      <c r="H114" s="9" t="n">
-        <v>3.03624</v>
-      </c>
-      <c r="I114" s="9" t="n">
-        <f aca="false">B114*H114</f>
-        <v>12.14496</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K114" s="2" t="s">
+      <c r="J110" s="19"/>
+      <c r="L110" s="20"/>
+    </row>
+    <row r="111" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F112" s="21" t="s">
         <v>468</v>
       </c>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="22" t="n">
+        <f aca="false">SUM(I108:I110,I102,I106,I104/100)</f>
+        <v>123.62519</v>
+      </c>
+      <c r="J112" s="23"/>
+    </row>
+    <row r="113" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="24" t="s">
+        <v>469</v>
+      </c>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+      <c r="I114" s="24"/>
     </row>
     <row r="115" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B115" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E115" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J115,J115)</f>
-        <v>ED2910-ND</v>
+        <v>ED1723-ND</v>
       </c>
       <c r="F115" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K115,K115)</f>
-        <v>538-39530-0004</v>
+        <v>538-39530-0008</v>
       </c>
       <c r="G115" s="2" t="n">
         <f aca="false">100*B115</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H115" s="9" t="n">
-        <v>1.197</v>
+        <v>3.03624</v>
       </c>
       <c r="I115" s="9" t="n">
         <f aca="false">B115*H115</f>
-        <v>2.394</v>
+        <v>12.14496</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B116" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E116" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J116,J116)</f>
-        <v>277-1101-ND</v>
+        <v>ED2910-ND</v>
       </c>
       <c r="F116" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K116,K116)</f>
-        <v>651-1757307</v>
+        <v>538-39530-0004</v>
       </c>
       <c r="G116" s="2" t="n">
         <f aca="false">100*B116</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H116" s="9" t="n">
-        <v>1.8674</v>
+        <v>1.197</v>
       </c>
       <c r="I116" s="9" t="n">
         <f aca="false">B116*H116</f>
-        <v>7.4696</v>
+        <v>2.394</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B117" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E117" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J117,J117)</f>
-        <v>A98067-ND</v>
+        <v>277-1101-ND</v>
       </c>
       <c r="F117" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K117,K117)</f>
-        <v>571-282814-4</v>
+        <v>651-1757307</v>
       </c>
       <c r="G117" s="2" t="n">
         <f aca="false">100*B117</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H117" s="9" t="n">
-        <v>0.794</v>
+        <v>1.8674</v>
       </c>
       <c r="I117" s="9" t="n">
         <f aca="false">B117*H117</f>
+        <v>7.4696</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="E118" s="8" t="str">
+        <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J118,J118)</f>
+        <v>A98067-ND</v>
+      </c>
+      <c r="F118" s="8" t="str">
+        <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K118,K118)</f>
+        <v>571-282814-4</v>
+      </c>
+      <c r="G118" s="2" t="n">
+        <f aca="false">100*B118</f>
+        <v>200</v>
+      </c>
+      <c r="H118" s="9" t="n">
+        <v>0.794</v>
+      </c>
+      <c r="I118" s="9" t="n">
+        <f aca="false">B118*H118</f>
         <v>1.588</v>
       </c>
-      <c r="J117" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
+      <c r="J118" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F119" s="25" t="s">
-        <v>455</v>
-      </c>
-      <c r="G119" s="25"/>
-      <c r="H119" s="25"/>
-      <c r="I119" s="9" t="n">
-        <f aca="false">SUM(I2:I29,I32:I100,I114:I117)</f>
-        <v>114.09786</v>
-      </c>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G120" s="17" t="s">
-        <v>481</v>
-      </c>
-      <c r="H120" s="17"/>
+      <c r="F120" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="G120" s="25"/>
+      <c r="H120" s="25"/>
       <c r="I120" s="9" t="n">
-        <f aca="false">I119-I101</f>
+        <f aca="false">SUM(I2:I29,I32:I101,I115:I118)</f>
+        <v>114.49786</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G121" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="H121" s="17"/>
+      <c r="I121" s="9" t="n">
+        <f aca="false">I120-I102</f>
         <v>19.80156</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-    </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H122" s="17" t="s">
-        <v>458</v>
-      </c>
-      <c r="I122" s="9" t="n">
-        <f aca="false">I104*(I119+I103/100)</f>
-        <v>34.349358</v>
-      </c>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
+      <c r="H123" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="I123" s="9" t="n">
+        <f aca="false">I105*(I120+I104/100)</f>
+        <v>34.469358</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F124" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="G124" s="21"/>
-      <c r="H124" s="21"/>
-      <c r="I124" s="22" t="n">
-        <f aca="false">SUM(I107:I109,I119,I122,I103/100)</f>
-        <v>148.847218</v>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F125" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="I125" s="22" t="n">
+        <f aca="false">SUM(I108:I110,I120,I123,I104/100)</f>
+        <v>149.367218</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="G104:H104"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="A113:I113"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="A114:I114"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="F125:H125"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
#8 corrected C80 Digi-Key code in BOM. Closed.
</commit_message>
<xml_diff>
--- a/PCB/NXP/docs/ciaa-nxp-bom.xlsx
+++ b/PCB/NXP/docs/ciaa-nxp-bom.xlsx
@@ -172,7 +172,7 @@
     <t>Cap. Tantáleo SMD</t>
   </si>
   <si>
-    <t>399-1086-1-ND</t>
+    <t>399-5502-1-ND</t>
   </si>
   <si>
     <t>80-C0603C335M9P</t>
@@ -1883,9 +1883,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>616680</xdr:colOff>
+      <xdr:colOff>617400</xdr:colOff>
       <xdr:row>100</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -1900,8 +1900,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8134200" y="20710800"/>
-          <a:ext cx="2530440" cy="1389240"/>
+          <a:off x="8134920" y="20711160"/>
+          <a:ext cx="2529720" cy="1388880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1946,8 +1946,8 @@
   </sheetPr>
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="E11" s="8" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.com/product-search/en?KeyWords="&amp;J11,J11)</f>
-        <v>399-1086-1-ND</v>
+        <v>399-5502-1-ND</v>
       </c>
       <c r="F11" s="8" t="str">
         <f aca="false">HYPERLINK("http://ar.mouser.com/Search/Refine.aspx?Keyword="&amp;K11,K11)</f>

</xml_diff>